<commit_message>
produce plots (w/errors) removed sim files
</commit_message>
<xml_diff>
--- a/config_randy.xlsx
+++ b/config_randy.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="188">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -143,21 +143,33 @@
     <t xml:space="preserve">m</t>
   </si>
   <si>
+    <t xml:space="preserve">length of vehicle</t>
+  </si>
+  <si>
     <t xml:space="preserve">g</t>
   </si>
   <si>
     <t xml:space="preserve">m/s^2</t>
   </si>
   <si>
+    <t xml:space="preserve">gravity constant</t>
+  </si>
+  <si>
     <t xml:space="preserve">a</t>
   </si>
   <si>
+    <t xml:space="preserve">acceleration</t>
+  </si>
+  <si>
     <t xml:space="preserve">xi</t>
   </si>
   <si>
     <t xml:space="preserve">deg/s</t>
   </si>
   <si>
+    <t xml:space="preserve">steering angle rate</t>
+  </si>
+  <si>
     <t xml:space="preserve">f</t>
   </si>
   <si>
@@ -170,27 +182,42 @@
     <t xml:space="preserve">r_body2antenna1_x</t>
   </si>
   <si>
+    <t xml:space="preserve">body to antenna one, x dimension</t>
+  </si>
+  <si>
     <t xml:space="preserve">r_body2antenna1_y</t>
   </si>
   <si>
+    <t xml:space="preserve">body to antenna one, y dimension</t>
+  </si>
+  <si>
     <t xml:space="preserve">r_body2antenna1_z</t>
   </si>
   <si>
+    <t xml:space="preserve">body to antenna one, z dimension</t>
+  </si>
+  <si>
     <t xml:space="preserve">r_body2antenna2_x</t>
   </si>
   <si>
+    <t xml:space="preserve">body to antenna two, x dimension</t>
+  </si>
+  <si>
     <t xml:space="preserve">r_body2antenna2_y</t>
   </si>
   <si>
+    <t xml:space="preserve">body to antenna two, y dimension</t>
+  </si>
+  <si>
     <t xml:space="preserve">r_body2antenna2_z</t>
   </si>
   <si>
+    <t xml:space="preserve">body to antenna two, z dimension</t>
+  </si>
+  <si>
     <t xml:space="preserve">nu</t>
   </si>
   <si>
-    <t xml:space="preserve">unitless?</t>
-  </si>
-  <si>
     <t xml:space="preserve">measurement noise</t>
   </si>
   <si>
@@ -201,6 +228,12 @@
   </si>
   <si>
     <t xml:space="preserve">speed of light</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">what is this about</t>
   </si>
   <si>
     <t xml:space="preserve">ri_x</t>
@@ -1147,10 +1180,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1426,6 +1459,9 @@
       <c r="C15" s="13" t="s">
         <v>34</v>
       </c>
+      <c r="D15" s="0" t="s">
+        <v>35</v>
+      </c>
       <c r="E15" s="2" t="n">
         <f aca="false">B15</f>
         <v>1.5</v>
@@ -1433,13 +1469,16 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>9.8</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>38</v>
       </c>
       <c r="E16" s="2" t="n">
         <f aca="false">B16</f>
@@ -1448,13 +1487,16 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>0.5</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>40</v>
       </c>
       <c r="E17" s="2" t="n">
         <f aca="false">B17</f>
@@ -1463,13 +1505,16 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>0.5</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>39</v>
+        <v>42</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>43</v>
       </c>
       <c r="E18" s="2" t="n">
         <f aca="false">RADIANS(B18)</f>
@@ -1478,25 +1523,25 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>1000000</v>
+        <v>24000000</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E19" s="2" t="n">
         <f aca="false">B19</f>
-        <v>1000000</v>
+        <v>24000000</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B20" s="1" t="n">
         <v>0</v>
@@ -1504,14 +1549,17 @@
       <c r="C20" s="0" t="s">
         <v>34</v>
       </c>
+      <c r="D20" s="0" t="s">
+        <v>48</v>
+      </c>
       <c r="E20" s="2" t="n">
-        <f aca="false">B19</f>
-        <v>1000000</v>
+        <f aca="false">B20</f>
+        <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="26" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B21" s="1" t="n">
         <f aca="false">1.5/4</f>
@@ -1520,6 +1568,9 @@
       <c r="C21" s="26" t="s">
         <v>34</v>
       </c>
+      <c r="D21" s="0" t="s">
+        <v>50</v>
+      </c>
       <c r="E21" s="2" t="n">
         <f aca="false">B20</f>
         <v>0</v>
@@ -1527,13 +1578,16 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="26" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>0</v>
       </c>
       <c r="C22" s="26" t="s">
         <v>34</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>52</v>
       </c>
       <c r="E22" s="2" t="n">
         <f aca="false">B21</f>
@@ -1542,7 +1596,7 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>0</v>
@@ -1550,6 +1604,9 @@
       <c r="C23" s="26" t="s">
         <v>34</v>
       </c>
+      <c r="D23" s="0" t="s">
+        <v>54</v>
+      </c>
       <c r="E23" s="2" t="n">
         <f aca="false">B22</f>
         <v>0</v>
@@ -1557,7 +1614,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="26" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B24" s="1" t="n">
         <f aca="false">-1.5/4</f>
@@ -1566,6 +1623,9 @@
       <c r="C24" s="26" t="s">
         <v>34</v>
       </c>
+      <c r="D24" s="0" t="s">
+        <v>56</v>
+      </c>
       <c r="E24" s="2" t="n">
         <f aca="false">B23</f>
         <v>0</v>
@@ -1573,13 +1633,16 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="26" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B25" s="1" t="n">
         <v>0</v>
       </c>
       <c r="C25" s="26" t="s">
         <v>34</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>58</v>
       </c>
       <c r="E25" s="2" t="n">
         <f aca="false">B24</f>
@@ -1588,16 +1651,16 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="B26" s="1" t="n">
         <v>0</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="E26" s="2" t="n">
         <f aca="false">B25</f>
@@ -1606,20 +1669,35 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="B27" s="1" t="n">
         <v>3335640000</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="E27" s="2" t="n">
         <f aca="false">B27</f>
         <v>3335640000</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="1" t="n">
+        <v>858</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <f aca="false">B283</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1652,7 +1730,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="B1" s="0" t="n">
         <v>60</v>
@@ -1660,7 +1738,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>173</v>
+        <v>184</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>60</v>
@@ -1668,7 +1746,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="B3" s="0" t="n">
         <f aca="false">hr2min*min2sec</f>
@@ -1677,7 +1755,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>9.81</v>
@@ -1685,7 +1763,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>24</v>
@@ -1742,7 +1820,7 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="31" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="B2" s="32" t="n">
         <v>0</v>
@@ -1751,7 +1829,7 @@
         <v>34</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="E2" s="35" t="n">
         <f aca="false">B2</f>
@@ -1760,7 +1838,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="36" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="B3" s="37" t="n">
         <v>0</v>
@@ -1769,7 +1847,7 @@
         <v>34</v>
       </c>
       <c r="D3" s="34" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="E3" s="39" t="n">
         <f aca="false">B3</f>
@@ -1778,16 +1856,16 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="40" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="B4" s="41" t="n">
         <v>10</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="E4" s="43" t="n">
         <f aca="false">B4</f>
@@ -1796,16 +1874,16 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="44" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="B5" s="41" t="n">
         <v>22.5</v>
       </c>
       <c r="C5" s="45" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="D5" s="42" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="E5" s="43" t="n">
         <f aca="false">RADIANS(B5)</f>
@@ -1814,16 +1892,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="44" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="B6" s="41" t="n">
         <v>-3</v>
       </c>
       <c r="C6" s="45" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="D6" s="42" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="E6" s="43" t="n">
         <f aca="false">RADIANS(B6)</f>
@@ -1832,16 +1910,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="46" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B7" s="32" t="n">
         <v>0</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="E7" s="35" t="n">
         <f aca="false">B7*g2mps2</f>
@@ -1850,16 +1928,16 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="47" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="B8" s="48" t="n">
         <v>0</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="E8" s="49" t="n">
         <f aca="false">B8*g2mps2</f>
@@ -1868,16 +1946,16 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="50" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="B9" s="51" t="n">
         <v>0</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D9" s="34" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="E9" s="39" t="n">
         <f aca="false">B9*g2mps2</f>
@@ -1886,16 +1964,16 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="52" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="B10" s="53" t="n">
         <v>0</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="E10" s="54" t="n">
         <f aca="false">RADIANS(B10)/hr2sec</f>
@@ -1904,16 +1982,16 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="52" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="B11" s="55" t="n">
         <v>0</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="E11" s="56" t="n">
         <f aca="false">RADIANS(B11)/hr2sec</f>
@@ -1922,16 +2000,16 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="52" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="B12" s="57" t="n">
         <v>0</v>
       </c>
       <c r="C12" s="38" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="E12" s="58" t="n">
         <f aca="false">RADIANS(B12)/hr2sec</f>
@@ -1940,7 +2018,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B13" s="53" t="n">
         <v>0</v>
@@ -1949,7 +2027,7 @@
         <v>34</v>
       </c>
       <c r="D13" s="33" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="E13" s="59" t="n">
         <f aca="false">B13</f>
@@ -1958,7 +2036,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="B14" s="55" t="n">
         <v>0</v>
@@ -1967,7 +2045,7 @@
         <v>34</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>82</v>
+        <v>93</v>
       </c>
       <c r="E14" s="60" t="n">
         <f aca="false">B14</f>
@@ -1976,7 +2054,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="61" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="B15" s="57" t="n">
         <v>0</v>
@@ -1985,7 +2063,7 @@
         <v>34</v>
       </c>
       <c r="D15" s="38" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="E15" s="63" t="n">
         <f aca="false">B15</f>
@@ -2025,24 +2103,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
@@ -2059,7 +2137,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>3</v>
@@ -2076,7 +2154,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>4</v>
@@ -2093,7 +2171,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>5</v>
@@ -2110,7 +2188,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="46" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>6</v>
@@ -2127,7 +2205,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>9</v>
@@ -2144,7 +2222,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>12</v>
@@ -2161,7 +2239,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>1</v>
@@ -2178,7 +2256,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>6</v>
@@ -2226,24 +2304,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
@@ -2260,7 +2338,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>4</v>
@@ -2277,7 +2355,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>7</v>
@@ -2294,7 +2372,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>11</v>
@@ -2311,7 +2389,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>14</v>
@@ -2328,7 +2406,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>17</v>
@@ -2345,7 +2423,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="B8" s="0" t="n">
         <f aca="false">B2</f>
@@ -2364,7 +2442,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="B9" s="0" t="n">
         <f aca="false">B5</f>
@@ -2434,17 +2512,17 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="69" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="B2" s="70" t="n">
         <f aca="false">0.00000016*3</f>
         <v>4.8E-007</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="E2" s="56" t="n">
         <f aca="false">B2/3</f>
@@ -2453,16 +2531,16 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="69" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="B3" s="71" t="n">
         <v>5</v>
       </c>
       <c r="C3" s="70" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="D3" s="34" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="E3" s="56" t="n">
         <f aca="false">RADIANS(B3)/hr2sec/3</f>
@@ -2472,16 +2550,16 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="36" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="B4" s="72" t="n">
         <v>0.05</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="D4" s="38" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="E4" s="58" t="n">
         <f aca="false">RADIANS(B4)/SQRT(hr2sec)/3</f>
@@ -2490,16 +2568,16 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="69" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="B5" s="71" t="n">
         <v>20</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="E5" s="56" t="n">
         <f aca="false">RADIANS(B5)/3600/3</f>
@@ -2508,16 +2586,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="69" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="B6" s="71" t="n">
         <v>20</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="E6" s="56" t="n">
         <f aca="false">RADIANS(B6)/3600/3</f>
@@ -2526,16 +2604,16 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="B7" s="71" t="n">
         <v>1.5</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="E7" s="56" t="n">
         <f aca="false">RADIANS(B7)/3600/3</f>
@@ -2544,16 +2622,16 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="B8" s="71" t="n">
         <v>1.5</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="E8" s="56" t="n">
         <f aca="false">RADIANS(B8)/3600/3</f>
@@ -2562,16 +2640,16 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="B9" s="71" t="n">
         <v>9</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="E9" s="56" t="n">
         <f aca="false">RADIANS(B9)/3600/3</f>
@@ -2580,16 +2658,16 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="B10" s="73" t="n">
         <v>3</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="E10" s="54" t="n">
         <f aca="false">B10/3</f>
@@ -2598,16 +2676,16 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="61" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="B11" s="74" t="n">
         <v>3</v>
       </c>
       <c r="C11" s="62" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="D11" s="62" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="E11" s="58" t="n">
         <f aca="false">B11/3</f>
@@ -2616,7 +2694,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="B12" s="64" t="n">
         <v>10</v>
@@ -2625,7 +2703,7 @@
         <v>34</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="E12" s="2" t="n">
         <f aca="false">B12/3</f>
@@ -2634,7 +2712,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="B13" s="64" t="n">
         <v>100</v>
@@ -2643,7 +2721,7 @@
         <v>34</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="E13" s="2" t="n">
         <f aca="false">B13/3</f>
@@ -2652,7 +2730,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="B14" s="64" t="n">
         <v>10</v>
@@ -2661,7 +2739,7 @@
         <v>34</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="E14" s="2" t="n">
         <f aca="false">B14/3</f>
@@ -2719,7 +2797,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="31" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="B2" s="33" t="n">
         <v>4000</v>
@@ -2728,7 +2806,7 @@
         <v>34</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="E2" s="54" t="n">
         <f aca="false">B2/3</f>
@@ -2737,7 +2815,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="69" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="B3" s="34" t="n">
         <v>4000</v>
@@ -2746,7 +2824,7 @@
         <v>34</v>
       </c>
       <c r="D3" s="34" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="E3" s="56" t="n">
         <f aca="false">B3/3</f>
@@ -2755,7 +2833,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="69" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="B4" s="34" t="n">
         <v>4000</v>
@@ -2764,7 +2842,7 @@
         <v>34</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="E4" s="56" t="n">
         <f aca="false">B4/3</f>
@@ -2773,16 +2851,16 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="69" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="B5" s="34" t="n">
         <v>3</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="E5" s="56" t="n">
         <f aca="false">B5/3</f>
@@ -2791,16 +2869,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="69" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="B6" s="34" t="n">
         <v>3</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="E6" s="56" t="n">
         <f aca="false">B6/3</f>
@@ -2809,16 +2887,16 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="69" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="B7" s="34" t="n">
         <v>3</v>
       </c>
       <c r="C7" s="34" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="E7" s="56" t="n">
         <f aca="false">B7/3</f>
@@ -2827,16 +2905,16 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="69" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="B8" s="34" t="n">
         <v>0.0005</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="E8" s="56" t="n">
         <f aca="false">B8/3</f>
@@ -2845,16 +2923,16 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="69" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="B9" s="34" t="n">
         <v>0.0005</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="D9" s="34" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="E9" s="56" t="n">
         <f aca="false">B9/3</f>
@@ -2863,16 +2941,16 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="69" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="B10" s="34" t="n">
         <v>0.0005</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="E10" s="56" t="n">
         <f aca="false">B10/3</f>
@@ -2881,17 +2959,17 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="69" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="B11" s="34" t="n">
         <f aca="false">truthStateParams!$B$5</f>
         <v>20</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="E11" s="56" t="n">
         <f aca="false">RADIANS(B11)/3600/3</f>
@@ -2900,17 +2978,17 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="B12" s="34" t="n">
         <f aca="false">truthStateParams!$B$5</f>
         <v>20</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="E12" s="56" t="n">
         <f aca="false">RADIANS(B12)/3600/3</f>
@@ -2919,17 +2997,17 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="B13" s="34" t="n">
         <f aca="false">truthStateParams!$B$5</f>
         <v>20</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="E13" s="56" t="n">
         <f aca="false">RADIANS(B13)/3600/3</f>
@@ -2938,17 +3016,17 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="B14" s="34" t="n">
         <f aca="false">truthStateParams!$B$6</f>
         <v>20</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="E14" s="56" t="n">
         <f aca="false">RADIANS(B14)/3600/3</f>
@@ -2957,17 +3035,17 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="B15" s="34" t="n">
         <f aca="false">truthStateParams!$B$6</f>
         <v>20</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="E15" s="56" t="n">
         <f aca="false">RADIANS(B15)/3600/3</f>
@@ -2976,17 +3054,17 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="13" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="B16" s="34" t="n">
         <f aca="false">truthStateParams!$B$6</f>
         <v>20</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="E16" s="56" t="n">
         <f aca="false">RADIANS(B16)/3600/3</f>
@@ -2995,17 +3073,17 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="69" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="B17" s="34" t="n">
         <f aca="false">truthStateParams!$B$3</f>
         <v>5</v>
       </c>
       <c r="C17" s="70" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="E17" s="56" t="n">
         <f aca="false">RADIANS(B17)/hr2sec/3</f>
@@ -3014,17 +3092,17 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="69" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="B18" s="34" t="n">
         <f aca="false">truthStateParams!$B$3</f>
         <v>5</v>
       </c>
       <c r="C18" s="70" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="D18" s="34" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="E18" s="56" t="n">
         <f aca="false">RADIANS(B18)/hr2sec/3</f>
@@ -3033,17 +3111,17 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="36" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="B19" s="38" t="n">
         <f aca="false">truthStateParams!$B$3</f>
         <v>5</v>
       </c>
       <c r="C19" s="76" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="D19" s="38" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="E19" s="58" t="n">
         <f aca="false">RADIANS(B19)/hr2sec/3</f>
@@ -3889,7 +3967,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="69" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="B2" s="34" t="n">
         <v>1</v>
@@ -3905,7 +3983,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="69" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="B3" s="34" t="n">
         <v>2</v>
@@ -3921,7 +3999,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="69" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="B4" s="34" t="n">
         <v>3</v>
@@ -3937,7 +4015,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="69" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="B5" s="34" t="n">
         <v>0.1</v>
@@ -3954,7 +4032,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="69" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="B6" s="34" t="n">
         <v>0.2</v>
@@ -3971,7 +4049,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="69" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="B7" s="34" t="n">
         <v>0.3</v>
@@ -3988,13 +4066,13 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="69" t="s">
-        <v>159</v>
+        <v>170</v>
       </c>
       <c r="B8" s="34" t="n">
         <v>0.11</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="D8" s="34"/>
       <c r="E8" s="79" t="n">
@@ -4004,13 +4082,13 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="69" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="B9" s="34" t="n">
         <v>0.22</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="D9" s="34"/>
       <c r="E9" s="79" t="n">
@@ -4020,13 +4098,13 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="69" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="B10" s="34" t="n">
         <v>0.33</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="D10" s="34"/>
       <c r="E10" s="79" t="n">
@@ -4036,13 +4114,13 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="69" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="B11" s="34" t="n">
         <v>0.001</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D11" s="34"/>
       <c r="E11" s="79" t="n">
@@ -4052,13 +4130,13 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="69" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="B12" s="34" t="n">
         <v>0.002</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D12" s="34"/>
       <c r="E12" s="79" t="n">
@@ -4068,13 +4146,13 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="69" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="B13" s="34" t="n">
         <v>0.003</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D13" s="34"/>
       <c r="E13" s="79" t="n">
@@ -4084,13 +4162,13 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="69" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="B14" s="34" t="n">
         <v>1.1</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="D14" s="34"/>
       <c r="E14" s="79" t="n">
@@ -4100,13 +4178,13 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="69" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="B15" s="34" t="n">
         <v>1.2</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="D15" s="34"/>
       <c r="E15" s="79" t="n">
@@ -4116,13 +4194,13 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="69" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="B16" s="34" t="n">
         <v>1.3</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="D16" s="34"/>
       <c r="E16" s="79" t="n">
@@ -4132,7 +4210,7 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="69" t="s">
-        <v>169</v>
+        <v>180</v>
       </c>
       <c r="B17" s="34" t="n">
         <v>0.01</v>
@@ -4148,7 +4226,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="69" t="s">
-        <v>170</v>
+        <v>181</v>
       </c>
       <c r="B18" s="34" t="n">
         <v>0.02</v>
@@ -4164,7 +4242,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="36" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="B19" s="38" t="n">
         <v>0.03</v>

</xml_diff>

<commit_message>
producing plots but the true trajectory and estimated trajectory or totally different
</commit_message>
<xml_diff>
--- a/config_randy.xlsx
+++ b/config_randy.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="177">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -143,33 +143,21 @@
     <t xml:space="preserve">m</t>
   </si>
   <si>
-    <t xml:space="preserve">length of vehicle</t>
-  </si>
-  <si>
     <t xml:space="preserve">g</t>
   </si>
   <si>
     <t xml:space="preserve">m/s^2</t>
   </si>
   <si>
-    <t xml:space="preserve">gravity constant</t>
-  </si>
-  <si>
     <t xml:space="preserve">a</t>
   </si>
   <si>
-    <t xml:space="preserve">acceleration</t>
-  </si>
-  <si>
     <t xml:space="preserve">xi</t>
   </si>
   <si>
     <t xml:space="preserve">deg/s</t>
   </si>
   <si>
-    <t xml:space="preserve">steering angle rate</t>
-  </si>
-  <si>
     <t xml:space="preserve">f</t>
   </si>
   <si>
@@ -182,42 +170,27 @@
     <t xml:space="preserve">r_body2antenna1_x</t>
   </si>
   <si>
-    <t xml:space="preserve">body to antenna one, x dimension</t>
-  </si>
-  <si>
     <t xml:space="preserve">r_body2antenna1_y</t>
   </si>
   <si>
-    <t xml:space="preserve">body to antenna one, y dimension</t>
-  </si>
-  <si>
     <t xml:space="preserve">r_body2antenna1_z</t>
   </si>
   <si>
-    <t xml:space="preserve">body to antenna one, z dimension</t>
-  </si>
-  <si>
     <t xml:space="preserve">r_body2antenna2_x</t>
   </si>
   <si>
-    <t xml:space="preserve">body to antenna two, x dimension</t>
-  </si>
-  <si>
     <t xml:space="preserve">r_body2antenna2_y</t>
   </si>
   <si>
-    <t xml:space="preserve">body to antenna two, y dimension</t>
-  </si>
-  <si>
     <t xml:space="preserve">r_body2antenna2_z</t>
   </si>
   <si>
-    <t xml:space="preserve">body to antenna two, z dimension</t>
-  </si>
-  <si>
     <t xml:space="preserve">nu</t>
   </si>
   <si>
+    <t xml:space="preserve">unitless?</t>
+  </si>
+  <si>
     <t xml:space="preserve">measurement noise</t>
   </si>
   <si>
@@ -228,12 +201,6 @@
   </si>
   <si>
     <t xml:space="preserve">speed of light</t>
-  </si>
-  <si>
-    <t xml:space="preserve">extra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">what is this about</t>
   </si>
   <si>
     <t xml:space="preserve">ri_x</t>
@@ -778,7 +745,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="80">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -880,10 +847,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1183,7 +1146,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1449,7 +1412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
         <v>33</v>
       </c>
@@ -1458,90 +1421,78 @@
       </c>
       <c r="C15" s="13" t="s">
         <v>34</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>35</v>
       </c>
       <c r="E15" s="2" t="n">
         <f aca="false">B15</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>9.8</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E16" s="2" t="n">
         <f aca="false">B16</f>
         <v>9.8</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>0.5</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E17" s="2" t="n">
         <f aca="false">B17</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>0.5</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E18" s="2" t="n">
         <f aca="false">RADIANS(B18)</f>
         <v>0.00872664625997165</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>24000000</v>
+        <v>1</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E19" s="2" t="n">
         <f aca="false">B19</f>
-        <v>24000000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B20" s="1" t="n">
         <v>0</v>
@@ -1549,27 +1500,21 @@
       <c r="C20" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="0" t="s">
-        <v>48</v>
-      </c>
       <c r="E20" s="2" t="n">
-        <f aca="false">B20</f>
-        <v>0</v>
+        <f aca="false">B19</f>
+        <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="26" t="s">
-        <v>49</v>
+      <c r="A21" s="0" t="s">
+        <v>44</v>
       </c>
       <c r="B21" s="1" t="n">
         <f aca="false">1.5/4</f>
         <v>0.375</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="0" t="s">
         <v>34</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>50</v>
       </c>
       <c r="E21" s="2" t="n">
         <f aca="false">B20</f>
@@ -1577,17 +1522,14 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="26" t="s">
-        <v>51</v>
+      <c r="A22" s="0" t="s">
+        <v>45</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="0" t="s">
         <v>34</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>52</v>
       </c>
       <c r="E22" s="2" t="n">
         <f aca="false">B21</f>
@@ -1596,16 +1538,13 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="0" t="s">
         <v>34</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>54</v>
       </c>
       <c r="E23" s="2" t="n">
         <f aca="false">B22</f>
@@ -1613,18 +1552,15 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="26" t="s">
-        <v>55</v>
+      <c r="A24" s="0" t="s">
+        <v>47</v>
       </c>
       <c r="B24" s="1" t="n">
         <f aca="false">-1.5/4</f>
         <v>-0.375</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="0" t="s">
         <v>34</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>56</v>
       </c>
       <c r="E24" s="2" t="n">
         <f aca="false">B23</f>
@@ -1632,17 +1568,14 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="26" t="s">
-        <v>57</v>
+      <c r="A25" s="0" t="s">
+        <v>48</v>
       </c>
       <c r="B25" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="0" t="s">
         <v>34</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>58</v>
       </c>
       <c r="E25" s="2" t="n">
         <f aca="false">B24</f>
@@ -1651,16 +1584,16 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B26" s="1" t="n">
         <v>0</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E26" s="2" t="n">
         <f aca="false">B25</f>
@@ -1669,37 +1602,23 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B27" s="1" t="n">
         <v>3335640000</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E27" s="2" t="n">
         <f aca="false">B27</f>
         <v>3335640000</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="B28" s="1" t="n">
-        <v>858</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="E28" s="2" t="n">
-        <f aca="false">B283</f>
-        <v>0</v>
-      </c>
-    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1730,7 +1649,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B1" s="0" t="n">
         <v>60</v>
@@ -1738,7 +1657,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>60</v>
@@ -1746,7 +1665,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="B3" s="0" t="n">
         <f aca="false">hr2min*min2sec</f>
@@ -1755,7 +1674,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>9.81</v>
@@ -1763,7 +1682,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>24</v>
@@ -1788,7 +1707,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1802,270 +1721,270 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="28" t="s">
+      <c r="A1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="29" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="B2" s="32" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" s="33" t="s">
+      <c r="A2" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="34" t="s">
-        <v>67</v>
-      </c>
-      <c r="E2" s="35" t="n">
+      <c r="D2" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="34" t="n">
         <f aca="false">B2</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="36" t="s">
-        <v>68</v>
-      </c>
-      <c r="B3" s="37" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" s="38" t="s">
+      <c r="A3" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="E3" s="39" t="n">
+      <c r="D3" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="38" t="n">
         <f aca="false">B3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="40" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4" s="41" t="n">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="40" t="n">
         <v>10</v>
       </c>
-      <c r="C4" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" s="42" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4" s="43" t="n">
+      <c r="C4" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="42" t="n">
         <f aca="false">B4</f>
         <v>10</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="44" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="41" t="n">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="40" t="n">
         <v>22.5</v>
       </c>
-      <c r="C5" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" s="42" t="s">
-        <v>74</v>
-      </c>
-      <c r="E5" s="43" t="n">
+      <c r="C5" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="42" t="n">
         <f aca="false">RADIANS(B5)</f>
         <v>0.392699081698724</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="44" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" s="41" t="n">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="40" t="n">
         <v>-3</v>
       </c>
-      <c r="C6" s="45" t="s">
-        <v>73</v>
-      </c>
-      <c r="D6" s="42" t="s">
-        <v>76</v>
-      </c>
-      <c r="E6" s="43" t="n">
+      <c r="C6" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="42" t="n">
         <f aca="false">RADIANS(B6)</f>
         <v>-0.0523598775598299</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="34" t="n">
+        <f aca="false">B7*g2mps2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="47" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="48" t="n">
+        <f aca="false">B8*g2mps2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="50" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="38" t="n">
+        <f aca="false">B9*g2mps2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="52" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="53" t="n">
+        <f aca="false">RADIANS(B10)/hr2sec</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="51" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="54" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="55" t="n">
+        <f aca="false">RADIANS(B11)/hr2sec</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="32" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="34" t="s">
+      <c r="B12" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="E7" s="35" t="n">
-        <f aca="false">B7*g2mps2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="47" t="s">
+      <c r="E12" s="57" t="n">
+        <f aca="false">RADIANS(B12)/hr2sec</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B8" s="48" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="E8" s="49" t="n">
-        <f aca="false">B8*g2mps2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="50" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" s="51" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="E9" s="39" t="n">
-        <f aca="false">B9*g2mps2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="52" t="s">
-        <v>83</v>
-      </c>
-      <c r="B10" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="D10" s="34" t="s">
-        <v>85</v>
-      </c>
-      <c r="E10" s="54" t="n">
-        <f aca="false">RADIANS(B10)/hr2sec</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="52" t="s">
-        <v>86</v>
-      </c>
-      <c r="B11" s="55" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="D11" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="E11" s="56" t="n">
-        <f aca="false">RADIANS(B11)/hr2sec</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="52" t="s">
-        <v>88</v>
-      </c>
-      <c r="B12" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" s="38" t="s">
-        <v>84</v>
-      </c>
-      <c r="D12" s="34" t="s">
-        <v>89</v>
-      </c>
-      <c r="E12" s="58" t="n">
-        <f aca="false">RADIANS(B12)/hr2sec</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="B13" s="53" t="n">
+      <c r="B13" s="52" t="n">
         <v>0</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="33" t="s">
-        <v>91</v>
-      </c>
-      <c r="E13" s="59" t="n">
+      <c r="D13" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="E13" s="58" t="n">
         <f aca="false">B13</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="B14" s="55" t="n">
+        <v>81</v>
+      </c>
+      <c r="B14" s="54" t="n">
         <v>0</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="34" t="s">
-        <v>93</v>
-      </c>
-      <c r="E14" s="60" t="n">
+      <c r="D14" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" s="59" t="n">
         <f aca="false">B14</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="61" t="s">
-        <v>94</v>
-      </c>
-      <c r="B15" s="57" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" s="62" t="s">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="56" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="38" t="s">
-        <v>95</v>
-      </c>
-      <c r="E15" s="63" t="n">
+      <c r="D15" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" s="62" t="n">
         <f aca="false">B15</f>
         <v>0</v>
       </c>
@@ -2103,24 +2022,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
@@ -2137,7 +2056,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>3</v>
@@ -2154,7 +2073,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>4</v>
@@ -2171,7 +2090,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>5</v>
@@ -2187,8 +2106,8 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="46" t="s">
-        <v>103</v>
+      <c r="A6" s="45" t="s">
+        <v>92</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>6</v>
@@ -2205,7 +2124,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>9</v>
@@ -2222,7 +2141,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>12</v>
@@ -2239,7 +2158,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>1</v>
@@ -2256,7 +2175,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>6</v>
@@ -2304,24 +2223,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
@@ -2338,7 +2257,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>4</v>
@@ -2355,7 +2274,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>7</v>
@@ -2372,7 +2291,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>11</v>
@@ -2389,7 +2308,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>14</v>
@@ -2406,7 +2325,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>17</v>
@@ -2423,7 +2342,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B8" s="0" t="n">
         <f aca="false">B2</f>
@@ -2442,7 +2361,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="B9" s="0" t="n">
         <f aca="false">B5</f>
@@ -2485,7 +2404,7 @@
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="64" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="63" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="48.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="14.71"/>
@@ -2494,216 +2413,216 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="65" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="66" t="s">
+      <c r="A1" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="67" t="s">
+      <c r="C1" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="67" t="s">
+      <c r="D1" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="68" t="s">
+      <c r="E1" s="67" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="69" t="s">
-        <v>109</v>
-      </c>
-      <c r="B2" s="70" t="n">
+      <c r="A2" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="69" t="n">
         <f aca="false">0.00000016*3</f>
         <v>4.8E-007</v>
       </c>
-      <c r="C2" s="34" t="s">
-        <v>110</v>
+      <c r="C2" s="33" t="s">
+        <v>99</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E2" s="56" t="n">
+        <v>100</v>
+      </c>
+      <c r="E2" s="55" t="n">
         <f aca="false">B2/3</f>
         <v>1.6E-007</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="69" t="s">
-        <v>112</v>
-      </c>
-      <c r="B3" s="71" t="n">
+      <c r="A3" s="68" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="70" t="n">
         <v>5</v>
       </c>
-      <c r="C3" s="70" t="s">
-        <v>84</v>
-      </c>
-      <c r="D3" s="34" t="s">
-        <v>113</v>
-      </c>
-      <c r="E3" s="56" t="n">
+      <c r="C3" s="69" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="55" t="n">
         <f aca="false">RADIANS(B3)/hr2sec/3</f>
         <v>8.08022801849227E-006</v>
       </c>
       <c r="F3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="36" t="s">
-        <v>114</v>
-      </c>
-      <c r="B4" s="72" t="n">
+      <c r="A4" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="71" t="n">
         <v>0.05</v>
       </c>
-      <c r="C4" s="38" t="s">
-        <v>115</v>
-      </c>
-      <c r="D4" s="38" t="s">
-        <v>116</v>
-      </c>
-      <c r="E4" s="58" t="n">
+      <c r="C4" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" s="57" t="n">
         <f aca="false">RADIANS(B4)/SQRT(hr2sec)/3</f>
         <v>4.84813681109536E-006</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="69" t="s">
-        <v>117</v>
-      </c>
-      <c r="B5" s="71" t="n">
+      <c r="A5" s="68" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="70" t="n">
         <v>20</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="E5" s="56" t="n">
+        <v>108</v>
+      </c>
+      <c r="E5" s="55" t="n">
         <f aca="false">RADIANS(B5)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="69" t="s">
-        <v>120</v>
-      </c>
-      <c r="B6" s="71" t="n">
+      <c r="A6" s="68" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="70" t="n">
         <v>20</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="E6" s="56" t="n">
+        <v>110</v>
+      </c>
+      <c r="E6" s="55" t="n">
         <f aca="false">RADIANS(B6)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="B7" s="71" t="n">
+        <v>111</v>
+      </c>
+      <c r="B7" s="70" t="n">
         <v>1.5</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="E7" s="56" t="n">
+        <v>113</v>
+      </c>
+      <c r="E7" s="55" t="n">
         <f aca="false">RADIANS(B7)/3600/3</f>
         <v>2.42406840554768E-006</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="B8" s="71" t="n">
+        <v>114</v>
+      </c>
+      <c r="B8" s="70" t="n">
         <v>1.5</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="E8" s="56" t="n">
+        <v>113</v>
+      </c>
+      <c r="E8" s="55" t="n">
         <f aca="false">RADIANS(B8)/3600/3</f>
         <v>2.42406840554768E-006</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="B9" s="71" t="n">
+        <v>115</v>
+      </c>
+      <c r="B9" s="70" t="n">
         <v>9</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="E9" s="56" t="n">
+        <v>113</v>
+      </c>
+      <c r="E9" s="55" t="n">
         <f aca="false">RADIANS(B9)/3600/3</f>
         <v>1.45444104332861E-005</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="B10" s="73" t="n">
+        <v>116</v>
+      </c>
+      <c r="B10" s="72" t="n">
         <v>3</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="E10" s="54" t="n">
+        <v>118</v>
+      </c>
+      <c r="E10" s="53" t="n">
         <f aca="false">B10/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="61" t="s">
-        <v>130</v>
-      </c>
-      <c r="B11" s="74" t="n">
+      <c r="A11" s="60" t="s">
+        <v>119</v>
+      </c>
+      <c r="B11" s="73" t="n">
         <v>3</v>
       </c>
-      <c r="C11" s="62" t="s">
-        <v>128</v>
-      </c>
-      <c r="D11" s="62" t="s">
-        <v>131</v>
-      </c>
-      <c r="E11" s="58" t="n">
+      <c r="C11" s="61" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11" s="61" t="s">
+        <v>120</v>
+      </c>
+      <c r="E11" s="57" t="n">
         <f aca="false">B11/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="B12" s="64" t="n">
+        <v>121</v>
+      </c>
+      <c r="B12" s="63" t="n">
         <v>10</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>34</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="E12" s="2" t="n">
         <f aca="false">B12/3</f>
@@ -2712,16 +2631,16 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="B13" s="64" t="n">
+        <v>123</v>
+      </c>
+      <c r="B13" s="63" t="n">
         <v>100</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>34</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="E13" s="2" t="n">
         <f aca="false">B13/3</f>
@@ -2730,16 +2649,16 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="B14" s="64" t="n">
+        <v>125</v>
+      </c>
+      <c r="B14" s="63" t="n">
         <v>10</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>34</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="E14" s="2" t="n">
         <f aca="false">B14/3</f>
@@ -2770,360 +2689,360 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="34" width="9.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="34" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="34" width="51.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="75" width="14.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="34" width="17.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="34" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="9.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="33" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="33" width="51.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="74" width="14.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="33" width="17.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="33" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="28" t="s">
+      <c r="A1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="29" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="31" t="s">
-        <v>138</v>
-      </c>
-      <c r="B2" s="33" t="n">
+      <c r="A2" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="32" t="n">
         <v>4000</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="33" t="s">
-        <v>139</v>
-      </c>
-      <c r="E2" s="54" t="n">
+      <c r="D2" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" s="53" t="n">
         <f aca="false">B2/3</f>
         <v>1333.33333333333</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="69" t="s">
-        <v>140</v>
-      </c>
-      <c r="B3" s="34" t="n">
+      <c r="A3" s="68" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="33" t="n">
         <v>4000</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="34" t="s">
-        <v>139</v>
-      </c>
-      <c r="E3" s="56" t="n">
+      <c r="D3" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" s="55" t="n">
         <f aca="false">B3/3</f>
         <v>1333.33333333333</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="69" t="s">
-        <v>141</v>
-      </c>
-      <c r="B4" s="34" t="n">
+      <c r="A4" s="68" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="33" t="n">
         <v>4000</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="34" t="s">
-        <v>139</v>
-      </c>
-      <c r="E4" s="56" t="n">
+      <c r="D4" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="E4" s="55" t="n">
         <f aca="false">B4/3</f>
         <v>1333.33333333333</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="69" t="s">
-        <v>142</v>
-      </c>
-      <c r="B5" s="34" t="n">
+      <c r="A5" s="68" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" s="33" t="n">
         <v>3</v>
       </c>
-      <c r="C5" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="D5" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="E5" s="56" t="n">
+      <c r="C5" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="E5" s="55" t="n">
         <f aca="false">B5/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="69" t="s">
-        <v>145</v>
-      </c>
-      <c r="B6" s="34" t="n">
+      <c r="A6" s="68" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="33" t="n">
         <v>3</v>
       </c>
-      <c r="C6" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="D6" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="E6" s="56" t="n">
+      <c r="C6" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="E6" s="55" t="n">
         <f aca="false">B6/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="69" t="s">
-        <v>146</v>
-      </c>
-      <c r="B7" s="34" t="n">
+      <c r="A7" s="68" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" s="33" t="n">
         <v>3</v>
       </c>
-      <c r="C7" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="D7" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="E7" s="56" t="n">
+      <c r="C7" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="D7" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="E7" s="55" t="n">
         <f aca="false">B7/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="69" t="s">
-        <v>147</v>
-      </c>
-      <c r="B8" s="34" t="n">
+      <c r="A8" s="68" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" s="33" t="n">
         <v>0.0005</v>
       </c>
-      <c r="C8" s="34" t="s">
-        <v>148</v>
-      </c>
-      <c r="D8" s="34" t="s">
-        <v>149</v>
-      </c>
-      <c r="E8" s="56" t="n">
+      <c r="C8" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="E8" s="55" t="n">
         <f aca="false">B8/3</f>
         <v>0.000166666666666667</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="69" t="s">
-        <v>150</v>
-      </c>
-      <c r="B9" s="34" t="n">
+      <c r="A9" s="68" t="s">
+        <v>139</v>
+      </c>
+      <c r="B9" s="33" t="n">
         <v>0.0005</v>
       </c>
-      <c r="C9" s="34" t="s">
-        <v>148</v>
-      </c>
-      <c r="D9" s="34" t="s">
-        <v>149</v>
-      </c>
-      <c r="E9" s="56" t="n">
+      <c r="C9" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="D9" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="E9" s="55" t="n">
         <f aca="false">B9/3</f>
         <v>0.000166666666666667</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="69" t="s">
-        <v>151</v>
-      </c>
-      <c r="B10" s="34" t="n">
+      <c r="A10" s="68" t="s">
+        <v>140</v>
+      </c>
+      <c r="B10" s="33" t="n">
         <v>0.0005</v>
       </c>
-      <c r="C10" s="34" t="s">
-        <v>148</v>
-      </c>
-      <c r="D10" s="34" t="s">
-        <v>149</v>
-      </c>
-      <c r="E10" s="56" t="n">
+      <c r="C10" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="E10" s="55" t="n">
         <f aca="false">B10/3</f>
         <v>0.000166666666666667</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="69" t="s">
-        <v>152</v>
-      </c>
-      <c r="B11" s="34" t="n">
+      <c r="A11" s="68" t="s">
+        <v>141</v>
+      </c>
+      <c r="B11" s="33" t="n">
         <f aca="false">truthStateParams!$B$5</f>
         <v>20</v>
       </c>
-      <c r="C11" s="34" t="s">
-        <v>123</v>
+      <c r="C11" s="33" t="s">
+        <v>112</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="E11" s="56" t="n">
+        <v>142</v>
+      </c>
+      <c r="E11" s="55" t="n">
         <f aca="false">RADIANS(B11)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="B12" s="34" t="n">
+        <v>143</v>
+      </c>
+      <c r="B12" s="33" t="n">
         <f aca="false">truthStateParams!$B$5</f>
         <v>20</v>
       </c>
-      <c r="C12" s="34" t="s">
-        <v>123</v>
+      <c r="C12" s="33" t="s">
+        <v>112</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="E12" s="56" t="n">
+        <v>142</v>
+      </c>
+      <c r="E12" s="55" t="n">
         <f aca="false">RADIANS(B12)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="B13" s="34" t="n">
+        <v>144</v>
+      </c>
+      <c r="B13" s="33" t="n">
         <f aca="false">truthStateParams!$B$5</f>
         <v>20</v>
       </c>
-      <c r="C13" s="34" t="s">
-        <v>123</v>
+      <c r="C13" s="33" t="s">
+        <v>112</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="E13" s="56" t="n">
+        <v>142</v>
+      </c>
+      <c r="E13" s="55" t="n">
         <f aca="false">RADIANS(B13)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="B14" s="34" t="n">
+        <v>145</v>
+      </c>
+      <c r="B14" s="33" t="n">
         <f aca="false">truthStateParams!$B$6</f>
         <v>20</v>
       </c>
-      <c r="C14" s="34" t="s">
-        <v>123</v>
+      <c r="C14" s="33" t="s">
+        <v>112</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="E14" s="56" t="n">
+        <v>146</v>
+      </c>
+      <c r="E14" s="55" t="n">
         <f aca="false">RADIANS(B14)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="B15" s="34" t="n">
+        <v>147</v>
+      </c>
+      <c r="B15" s="33" t="n">
         <f aca="false">truthStateParams!$B$6</f>
         <v>20</v>
       </c>
-      <c r="C15" s="34" t="s">
-        <v>123</v>
+      <c r="C15" s="33" t="s">
+        <v>112</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="E15" s="56" t="n">
+        <v>146</v>
+      </c>
+      <c r="E15" s="55" t="n">
         <f aca="false">RADIANS(B15)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="B16" s="34" t="n">
+        <v>148</v>
+      </c>
+      <c r="B16" s="33" t="n">
         <f aca="false">truthStateParams!$B$6</f>
         <v>20</v>
       </c>
-      <c r="C16" s="34" t="s">
-        <v>123</v>
+      <c r="C16" s="33" t="s">
+        <v>112</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="E16" s="56" t="n">
+        <v>146</v>
+      </c>
+      <c r="E16" s="55" t="n">
         <f aca="false">RADIANS(B16)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="69" t="s">
-        <v>160</v>
-      </c>
-      <c r="B17" s="34" t="n">
+      <c r="A17" s="68" t="s">
+        <v>149</v>
+      </c>
+      <c r="B17" s="33" t="n">
         <f aca="false">truthStateParams!$B$3</f>
         <v>5</v>
       </c>
-      <c r="C17" s="70" t="s">
-        <v>84</v>
-      </c>
-      <c r="D17" s="34" t="s">
-        <v>161</v>
-      </c>
-      <c r="E17" s="56" t="n">
+      <c r="C17" s="69" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>150</v>
+      </c>
+      <c r="E17" s="55" t="n">
         <f aca="false">RADIANS(B17)/hr2sec/3</f>
         <v>8.08022801849227E-006</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="69" t="s">
-        <v>162</v>
-      </c>
-      <c r="B18" s="34" t="n">
+      <c r="A18" s="68" t="s">
+        <v>151</v>
+      </c>
+      <c r="B18" s="33" t="n">
         <f aca="false">truthStateParams!$B$3</f>
         <v>5</v>
       </c>
-      <c r="C18" s="70" t="s">
-        <v>84</v>
-      </c>
-      <c r="D18" s="34" t="s">
-        <v>161</v>
-      </c>
-      <c r="E18" s="56" t="n">
+      <c r="C18" s="69" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>150</v>
+      </c>
+      <c r="E18" s="55" t="n">
         <f aca="false">RADIANS(B18)/hr2sec/3</f>
         <v>8.08022801849227E-006</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="36" t="s">
-        <v>163</v>
-      </c>
-      <c r="B19" s="38" t="n">
+      <c r="A19" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="B19" s="37" t="n">
         <f aca="false">truthStateParams!$B$3</f>
         <v>5</v>
       </c>
-      <c r="C19" s="76" t="s">
-        <v>84</v>
-      </c>
-      <c r="D19" s="38" t="s">
-        <v>161</v>
-      </c>
-      <c r="E19" s="58" t="n">
+      <c r="C19" s="75" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="37" t="s">
+        <v>150</v>
+      </c>
+      <c r="E19" s="57" t="n">
         <f aca="false">RADIANS(B19)/hr2sec/3</f>
         <v>8.08022801849227E-006</v>
       </c>
@@ -3152,42 +3071,42 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="34" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="77" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="34" width="11.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="34" width="46.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="75" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="34" width="25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="34" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="76" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="33" width="11.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="33" width="46.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="74" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="33" width="25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="33" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="65" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="66" t="s">
+      <c r="A1" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="67" t="s">
+      <c r="C1" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="67" t="s">
+      <c r="D1" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="68" t="s">
+      <c r="E1" s="67" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="69" t="str">
+      <c r="A2" s="68" t="str">
         <f aca="false">truthStateParams!A2</f>
         <v>Q_grav</v>
       </c>
-      <c r="B2" s="70" t="n">
+      <c r="B2" s="69" t="n">
         <f aca="false">truthStateParams!B2</f>
         <v>4.8E-007</v>
       </c>
-      <c r="C2" s="34" t="str">
+      <c r="C2" s="33" t="str">
         <f aca="false">truthStateParams!C2</f>
         <v>m^2/s^3</v>
       </c>
@@ -3195,64 +3114,64 @@
         <f aca="false">truthStateParams!D2</f>
         <v>3-sigma non-gravitational process noise</v>
       </c>
-      <c r="E2" s="56" t="n">
+      <c r="E2" s="55" t="n">
         <f aca="false">B2/3</f>
         <v>1.6E-007</v>
       </c>
-      <c r="F2" s="75"/>
+      <c r="F2" s="74"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="69" t="str">
+      <c r="A3" s="68" t="str">
         <f aca="false">truthStateParams!A3</f>
         <v>sig_gyro_ss</v>
       </c>
-      <c r="B3" s="71" t="n">
+      <c r="B3" s="70" t="n">
         <f aca="false">truthStateParams!B3</f>
         <v>5</v>
       </c>
-      <c r="C3" s="70" t="str">
+      <c r="C3" s="69" t="str">
         <f aca="false">truthStateParams!C3</f>
         <v>deg/hr</v>
       </c>
-      <c r="D3" s="34" t="str">
+      <c r="D3" s="33" t="str">
         <f aca="false">truthStateParams!D3</f>
         <v>3-sigma steady-state gyro bias</v>
       </c>
-      <c r="E3" s="56" t="n">
+      <c r="E3" s="55" t="n">
         <f aca="false">RADIANS(B3)/hr2sec/3</f>
         <v>8.08022801849227E-006</v>
       </c>
-      <c r="F3" s="75"/>
+      <c r="F3" s="74"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="36" t="str">
+      <c r="A4" s="35" t="str">
         <f aca="false">truthStateParams!A4</f>
         <v>arw</v>
       </c>
-      <c r="B4" s="72" t="n">
+      <c r="B4" s="71" t="n">
         <f aca="false">truthStateParams!B4</f>
         <v>0.05</v>
       </c>
-      <c r="C4" s="38" t="str">
+      <c r="C4" s="37" t="str">
         <f aca="false">truthStateParams!C4</f>
         <v>deg/sqrt(hr)</v>
       </c>
-      <c r="D4" s="38" t="str">
+      <c r="D4" s="37" t="str">
         <f aca="false">truthStateParams!D4</f>
         <v>3-sigma angular random walk</v>
       </c>
-      <c r="E4" s="58" t="n">
+      <c r="E4" s="57" t="n">
         <f aca="false">RADIANS(B4)/SQRT(hr2sec)/3</f>
         <v>4.84813681109536E-006</v>
       </c>
-      <c r="F4" s="75"/>
+      <c r="F4" s="74"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="69" t="str">
+      <c r="A5" s="68" t="str">
         <f aca="false">truthStateParams!A5</f>
         <v>sig_st_ss</v>
       </c>
-      <c r="B5" s="71" t="n">
+      <c r="B5" s="70" t="n">
         <f aca="false">truthStateParams!B5</f>
         <v>20</v>
       </c>
@@ -3264,18 +3183,18 @@
         <f aca="false">truthStateParams!D5</f>
         <v>3-sigma steady-state star camera misalignment</v>
       </c>
-      <c r="E5" s="56" t="n">
+      <c r="E5" s="55" t="n">
         <f aca="false">RADIANS(B5)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
-      <c r="F5" s="75"/>
+      <c r="F5" s="74"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="69" t="str">
+      <c r="A6" s="68" t="str">
         <f aca="false">truthStateParams!A6</f>
         <v>sig_c_ss</v>
       </c>
-      <c r="B6" s="71" t="n">
+      <c r="B6" s="70" t="n">
         <f aca="false">truthStateParams!B6</f>
         <v>20</v>
       </c>
@@ -3287,7 +3206,7 @@
         <f aca="false">truthStateParams!D6</f>
         <v>3-sigma steady-state terrain camera misalignment</v>
       </c>
-      <c r="E6" s="56" t="n">
+      <c r="E6" s="55" t="n">
         <f aca="false">RADIANS(B6)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
@@ -3297,7 +3216,7 @@
         <f aca="false">truthStateParams!A7</f>
         <v>sig_meas_stx</v>
       </c>
-      <c r="B7" s="71" t="n">
+      <c r="B7" s="70" t="n">
         <f aca="false">truthStateParams!B7</f>
         <v>1.5</v>
       </c>
@@ -3309,7 +3228,7 @@
         <f aca="false">truthStateParams!D7</f>
         <v>3-sigma star camera measurement uncertainty</v>
       </c>
-      <c r="E7" s="56" t="n">
+      <c r="E7" s="55" t="n">
         <f aca="false">RADIANS(B7)/3600/3</f>
         <v>2.42406840554768E-006</v>
       </c>
@@ -3319,7 +3238,7 @@
         <f aca="false">truthStateParams!A8</f>
         <v>sig_meas_sty</v>
       </c>
-      <c r="B8" s="71" t="n">
+      <c r="B8" s="70" t="n">
         <f aca="false">truthStateParams!B8</f>
         <v>1.5</v>
       </c>
@@ -3331,7 +3250,7 @@
         <f aca="false">truthStateParams!D8</f>
         <v>3-sigma star camera measurement uncertainty</v>
       </c>
-      <c r="E8" s="56" t="n">
+      <c r="E8" s="55" t="n">
         <f aca="false">RADIANS(B8)/3600/3</f>
         <v>2.42406840554768E-006</v>
       </c>
@@ -3341,7 +3260,7 @@
         <f aca="false">truthStateParams!A9</f>
         <v>sig_meas_stz</v>
       </c>
-      <c r="B9" s="71" t="n">
+      <c r="B9" s="70" t="n">
         <f aca="false">truthStateParams!B9</f>
         <v>9</v>
       </c>
@@ -3353,7 +3272,7 @@
         <f aca="false">truthStateParams!D9</f>
         <v>3-sigma star camera measurement uncertainty</v>
       </c>
-      <c r="E9" s="56" t="n">
+      <c r="E9" s="55" t="n">
         <f aca="false">RADIANS(B9)/3600/3</f>
         <v>1.45444104332861E-005</v>
       </c>
@@ -3363,7 +3282,7 @@
         <f aca="false">truthStateParams!A10</f>
         <v>sig_cu</v>
       </c>
-      <c r="B10" s="73" t="n">
+      <c r="B10" s="72" t="n">
         <f aca="false">truthStateParams!B10</f>
         <v>3</v>
       </c>
@@ -3375,95 +3294,95 @@
         <f aca="false">truthStateParams!D10</f>
         <v>3-sigma u component of pixel noise</v>
       </c>
-      <c r="E10" s="54" t="n">
+      <c r="E10" s="53" t="n">
         <f aca="false">B10/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="61" t="str">
+      <c r="A11" s="60" t="str">
         <f aca="false">truthStateParams!A11</f>
         <v>sig_cv</v>
       </c>
-      <c r="B11" s="74" t="n">
+      <c r="B11" s="73" t="n">
         <f aca="false">truthStateParams!B11</f>
         <v>3</v>
       </c>
-      <c r="C11" s="62" t="str">
+      <c r="C11" s="61" t="str">
         <f aca="false">truthStateParams!C11</f>
         <v>pixels</v>
       </c>
-      <c r="D11" s="62" t="str">
+      <c r="D11" s="61" t="str">
         <f aca="false">truthStateParams!D11</f>
         <v>3-sigma v component of pixel noise</v>
       </c>
-      <c r="E11" s="58" t="n">
+      <c r="E11" s="57" t="n">
         <f aca="false">B11/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="61" t="str">
+      <c r="A12" s="60" t="str">
         <f aca="false">truthStateParams!A12</f>
         <v>sig_idpos</v>
       </c>
-      <c r="B12" s="74" t="n">
+      <c r="B12" s="73" t="n">
         <f aca="false">truthStateParams!B12</f>
         <v>10</v>
       </c>
-      <c r="C12" s="62" t="str">
+      <c r="C12" s="61" t="str">
         <f aca="false">truthStateParams!C12</f>
         <v>m</v>
       </c>
-      <c r="D12" s="62" t="str">
+      <c r="D12" s="61" t="str">
         <f aca="false">truthStateParams!D12</f>
         <v>3-sigma change in inertial position measurement uncertainty</v>
       </c>
-      <c r="E12" s="58" t="n">
+      <c r="E12" s="57" t="n">
         <f aca="false">B12/3</f>
         <v>3.33333333333333</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="61" t="str">
+      <c r="A13" s="60" t="str">
         <f aca="false">truthStateParams!A13</f>
         <v>sig_loss</v>
       </c>
-      <c r="B13" s="74" t="n">
+      <c r="B13" s="73" t="n">
         <f aca="false">truthStateParams!B13</f>
         <v>100</v>
       </c>
-      <c r="C13" s="62" t="str">
+      <c r="C13" s="61" t="str">
         <f aca="false">truthStateParams!C13</f>
         <v>m</v>
       </c>
-      <c r="D13" s="62" t="str">
+      <c r="D13" s="61" t="str">
         <f aca="false">truthStateParams!D13</f>
         <v>3-sigma LOSS feature location uncertainty</v>
       </c>
-      <c r="E13" s="58" t="n">
+      <c r="E13" s="57" t="n">
         <f aca="false">B13/3</f>
         <v>33.3333333333333</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="61" t="str">
+      <c r="A14" s="60" t="str">
         <f aca="false">truthStateParams!A14</f>
         <v>sig_mdpos</v>
       </c>
-      <c r="B14" s="74" t="n">
+      <c r="B14" s="73" t="n">
         <f aca="false">truthStateParams!B14</f>
         <v>10</v>
       </c>
-      <c r="C14" s="62" t="str">
+      <c r="C14" s="61" t="str">
         <f aca="false">truthStateParams!C14</f>
         <v>m</v>
       </c>
-      <c r="D14" s="62" t="str">
+      <c r="D14" s="61" t="str">
         <f aca="false">truthStateParams!D14</f>
         <v>3-sigma change in lunar-referenced position measurement uncertainty</v>
       </c>
-      <c r="E14" s="58" t="n">
+      <c r="E14" s="57" t="n">
         <f aca="false">B14/3</f>
         <v>3.33333333333333</v>
       </c>
@@ -3492,427 +3411,427 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="34" width="9.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="34" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="34" width="51.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="75" width="13.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="34" width="14.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="34" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="9.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="33" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="33" width="51.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="74" width="13.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="33" width="14.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="33" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="65" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="78" t="s">
+      <c r="A1" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="67" t="s">
+      <c r="C1" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="67" t="s">
+      <c r="D1" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="29" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="69" t="str">
+      <c r="A2" s="68" t="str">
         <f aca="false">truthStateInitialUncertainty!A2</f>
         <v>sig_rsx</v>
       </c>
-      <c r="B2" s="34" t="n">
+      <c r="B2" s="33" t="n">
         <f aca="false">truthStateInitialUncertainty!B2</f>
         <v>4000</v>
       </c>
-      <c r="C2" s="34" t="str">
+      <c r="C2" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!C2</f>
         <v>m</v>
       </c>
-      <c r="D2" s="34" t="str">
+      <c r="D2" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!D2</f>
         <v>3-sigma initial satellite position uncertainty</v>
       </c>
-      <c r="E2" s="79" t="n">
+      <c r="E2" s="78" t="n">
         <f aca="false">B2/3</f>
         <v>1333.33333333333</v>
       </c>
-      <c r="F2" s="75"/>
+      <c r="F2" s="74"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="69" t="str">
+      <c r="A3" s="68" t="str">
         <f aca="false">truthStateInitialUncertainty!A3</f>
         <v>sig_rsy</v>
       </c>
-      <c r="B3" s="34" t="n">
+      <c r="B3" s="33" t="n">
         <f aca="false">truthStateInitialUncertainty!B3</f>
         <v>4000</v>
       </c>
-      <c r="C3" s="34" t="str">
+      <c r="C3" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!C3</f>
         <v>m</v>
       </c>
-      <c r="D3" s="34" t="str">
+      <c r="D3" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!D3</f>
         <v>3-sigma initial satellite position uncertainty</v>
       </c>
-      <c r="E3" s="79" t="n">
+      <c r="E3" s="78" t="n">
         <f aca="false">B3/3</f>
         <v>1333.33333333333</v>
       </c>
-      <c r="F3" s="75"/>
+      <c r="F3" s="74"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="69" t="str">
+      <c r="A4" s="68" t="str">
         <f aca="false">truthStateInitialUncertainty!A4</f>
         <v>sig_rsz</v>
       </c>
-      <c r="B4" s="34" t="n">
+      <c r="B4" s="33" t="n">
         <f aca="false">truthStateInitialUncertainty!B4</f>
         <v>4000</v>
       </c>
-      <c r="C4" s="34" t="str">
+      <c r="C4" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!C4</f>
         <v>m</v>
       </c>
-      <c r="D4" s="34" t="str">
+      <c r="D4" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!D4</f>
         <v>3-sigma initial satellite position uncertainty</v>
       </c>
-      <c r="E4" s="79" t="n">
+      <c r="E4" s="78" t="n">
         <f aca="false">B4/3</f>
         <v>1333.33333333333</v>
       </c>
-      <c r="F4" s="75"/>
+      <c r="F4" s="74"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="69" t="str">
+      <c r="A5" s="68" t="str">
         <f aca="false">truthStateInitialUncertainty!A5</f>
         <v>sig_vsx</v>
       </c>
-      <c r="B5" s="34" t="n">
+      <c r="B5" s="33" t="n">
         <f aca="false">truthStateInitialUncertainty!B5</f>
         <v>3</v>
       </c>
-      <c r="C5" s="34" t="str">
+      <c r="C5" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!C5</f>
         <v>m/sec</v>
       </c>
-      <c r="D5" s="34" t="str">
+      <c r="D5" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!D5</f>
         <v>3-sigma initial satellite velocity uncertainty</v>
       </c>
-      <c r="E5" s="79" t="n">
+      <c r="E5" s="78" t="n">
         <f aca="false">B5/3</f>
         <v>1</v>
       </c>
-      <c r="F5" s="75"/>
+      <c r="F5" s="74"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="69" t="str">
+      <c r="A6" s="68" t="str">
         <f aca="false">truthStateInitialUncertainty!A6</f>
         <v>sig_vsy</v>
       </c>
-      <c r="B6" s="34" t="n">
+      <c r="B6" s="33" t="n">
         <f aca="false">truthStateInitialUncertainty!B6</f>
         <v>3</v>
       </c>
-      <c r="C6" s="34" t="str">
+      <c r="C6" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!C6</f>
         <v>m/sec</v>
       </c>
-      <c r="D6" s="34" t="str">
+      <c r="D6" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!D6</f>
         <v>3-sigma initial satellite velocity uncertainty</v>
       </c>
-      <c r="E6" s="79" t="n">
+      <c r="E6" s="78" t="n">
         <f aca="false">B6/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="69" t="str">
+      <c r="A7" s="68" t="str">
         <f aca="false">truthStateInitialUncertainty!A7</f>
         <v>sig_vsz</v>
       </c>
-      <c r="B7" s="34" t="n">
+      <c r="B7" s="33" t="n">
         <f aca="false">truthStateInitialUncertainty!B7</f>
         <v>3</v>
       </c>
-      <c r="C7" s="34" t="str">
+      <c r="C7" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!C7</f>
         <v>m/sec</v>
       </c>
-      <c r="D7" s="34" t="str">
+      <c r="D7" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!D7</f>
         <v>3-sigma initial satellite velocity uncertainty</v>
       </c>
-      <c r="E7" s="79" t="n">
+      <c r="E7" s="78" t="n">
         <f aca="false">B7/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="69" t="str">
+      <c r="A8" s="68" t="str">
         <f aca="false">truthStateInitialUncertainty!A8</f>
         <v>sig_ax</v>
       </c>
-      <c r="B8" s="34" t="n">
+      <c r="B8" s="33" t="n">
         <f aca="false">truthStateInitialUncertainty!B8</f>
         <v>0.0005</v>
       </c>
-      <c r="C8" s="34" t="str">
+      <c r="C8" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!C8</f>
         <v>rad</v>
       </c>
-      <c r="D8" s="34" t="str">
+      <c r="D8" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!D8</f>
         <v>3-sigma initial satellite orientation uncertainty</v>
       </c>
-      <c r="E8" s="79" t="n">
+      <c r="E8" s="78" t="n">
         <f aca="false">B8/3</f>
         <v>0.000166666666666667</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="69" t="str">
+      <c r="A9" s="68" t="str">
         <f aca="false">truthStateInitialUncertainty!A9</f>
         <v>sig_ay</v>
       </c>
-      <c r="B9" s="34" t="n">
+      <c r="B9" s="33" t="n">
         <f aca="false">truthStateInitialUncertainty!B9</f>
         <v>0.0005</v>
       </c>
-      <c r="C9" s="34" t="str">
+      <c r="C9" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!C9</f>
         <v>rad</v>
       </c>
-      <c r="D9" s="34" t="str">
+      <c r="D9" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!D9</f>
         <v>3-sigma initial satellite orientation uncertainty</v>
       </c>
-      <c r="E9" s="79" t="n">
+      <c r="E9" s="78" t="n">
         <f aca="false">B9/3</f>
         <v>0.000166666666666667</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="69" t="str">
+      <c r="A10" s="68" t="str">
         <f aca="false">truthStateInitialUncertainty!A10</f>
         <v>sig_az</v>
       </c>
-      <c r="B10" s="34" t="n">
+      <c r="B10" s="33" t="n">
         <f aca="false">truthStateInitialUncertainty!B10</f>
         <v>0.0005</v>
       </c>
-      <c r="C10" s="34" t="str">
+      <c r="C10" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!C10</f>
         <v>rad</v>
       </c>
-      <c r="D10" s="34" t="str">
+      <c r="D10" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!D10</f>
         <v>3-sigma initial satellite orientation uncertainty</v>
       </c>
-      <c r="E10" s="79" t="n">
+      <c r="E10" s="78" t="n">
         <f aca="false">B10/3</f>
         <v>0.000166666666666667</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="69" t="str">
+      <c r="A11" s="68" t="str">
         <f aca="false">truthStateInitialUncertainty!A11</f>
         <v>sig_thstx</v>
       </c>
-      <c r="B11" s="34" t="n">
+      <c r="B11" s="33" t="n">
         <f aca="false">truthStateInitialUncertainty!B11</f>
         <v>20</v>
       </c>
-      <c r="C11" s="34" t="str">
+      <c r="C11" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!C11</f>
         <v>arcsec</v>
       </c>
-      <c r="D11" s="34" t="str">
+      <c r="D11" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!D11</f>
         <v>3-sigma initial star camera misalignment uncertainty</v>
       </c>
-      <c r="E11" s="79" t="n">
+      <c r="E11" s="78" t="n">
         <f aca="false">RADIANS(B11)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="69" t="str">
+      <c r="A12" s="68" t="str">
         <f aca="false">truthStateInitialUncertainty!A12</f>
         <v>sig_thsty</v>
       </c>
-      <c r="B12" s="34" t="n">
+      <c r="B12" s="33" t="n">
         <f aca="false">truthStateInitialUncertainty!B12</f>
         <v>20</v>
       </c>
-      <c r="C12" s="34" t="str">
+      <c r="C12" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!C12</f>
         <v>arcsec</v>
       </c>
-      <c r="D12" s="34" t="str">
+      <c r="D12" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!D12</f>
         <v>3-sigma initial star camera misalignment uncertainty</v>
       </c>
-      <c r="E12" s="79" t="n">
+      <c r="E12" s="78" t="n">
         <f aca="false">RADIANS(B12)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="69" t="str">
+      <c r="A13" s="68" t="str">
         <f aca="false">truthStateInitialUncertainty!A13</f>
         <v>sig_thstz</v>
       </c>
-      <c r="B13" s="34" t="n">
+      <c r="B13" s="33" t="n">
         <f aca="false">truthStateInitialUncertainty!B13</f>
         <v>20</v>
       </c>
-      <c r="C13" s="34" t="str">
+      <c r="C13" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!C13</f>
         <v>arcsec</v>
       </c>
-      <c r="D13" s="34" t="str">
+      <c r="D13" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!D13</f>
         <v>3-sigma initial star camera misalignment uncertainty</v>
       </c>
-      <c r="E13" s="79" t="n">
+      <c r="E13" s="78" t="n">
         <f aca="false">RADIANS(B13)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="69" t="str">
+      <c r="A14" s="68" t="str">
         <f aca="false">truthStateInitialUncertainty!A14</f>
         <v>sig_thcx</v>
       </c>
-      <c r="B14" s="34" t="n">
+      <c r="B14" s="33" t="n">
         <f aca="false">truthStateInitialUncertainty!B14</f>
         <v>20</v>
       </c>
-      <c r="C14" s="34" t="str">
+      <c r="C14" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!C14</f>
         <v>arcsec</v>
       </c>
-      <c r="D14" s="34" t="str">
+      <c r="D14" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!D14</f>
         <v>3-sigma initial terrain camera misalignment uncertainty</v>
       </c>
-      <c r="E14" s="79" t="n">
+      <c r="E14" s="78" t="n">
         <f aca="false">RADIANS(B14)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="69" t="str">
+      <c r="A15" s="68" t="str">
         <f aca="false">truthStateInitialUncertainty!A15</f>
         <v>sig_thcy</v>
       </c>
-      <c r="B15" s="34" t="n">
+      <c r="B15" s="33" t="n">
         <f aca="false">truthStateInitialUncertainty!B15</f>
         <v>20</v>
       </c>
-      <c r="C15" s="34" t="str">
+      <c r="C15" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!C15</f>
         <v>arcsec</v>
       </c>
-      <c r="D15" s="34" t="str">
+      <c r="D15" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!D15</f>
         <v>3-sigma initial terrain camera misalignment uncertainty</v>
       </c>
-      <c r="E15" s="79" t="n">
+      <c r="E15" s="78" t="n">
         <f aca="false">RADIANS(B15)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="69" t="str">
+      <c r="A16" s="68" t="str">
         <f aca="false">truthStateInitialUncertainty!A16</f>
         <v>sig_thcz</v>
       </c>
-      <c r="B16" s="34" t="n">
+      <c r="B16" s="33" t="n">
         <f aca="false">truthStateInitialUncertainty!B16</f>
         <v>20</v>
       </c>
-      <c r="C16" s="34" t="str">
+      <c r="C16" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!C16</f>
         <v>arcsec</v>
       </c>
-      <c r="D16" s="34" t="str">
+      <c r="D16" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!D16</f>
         <v>3-sigma initial terrain camera misalignment uncertainty</v>
       </c>
-      <c r="E16" s="79" t="n">
+      <c r="E16" s="78" t="n">
         <f aca="false">RADIANS(B16)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="69" t="str">
+      <c r="A17" s="68" t="str">
         <f aca="false">truthStateInitialUncertainty!A17</f>
         <v>sig_gyrox</v>
       </c>
-      <c r="B17" s="34" t="n">
+      <c r="B17" s="33" t="n">
         <f aca="false">truthStateInitialUncertainty!B17</f>
         <v>5</v>
       </c>
-      <c r="C17" s="34" t="str">
+      <c r="C17" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!C17</f>
         <v>deg/hr</v>
       </c>
-      <c r="D17" s="34" t="str">
+      <c r="D17" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!D17</f>
         <v>3-sigma initial gyro bias uncertainty</v>
       </c>
-      <c r="E17" s="79" t="n">
+      <c r="E17" s="78" t="n">
         <f aca="false">RADIANS(B17)/hr2sec/3</f>
         <v>8.08022801849227E-006</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="69" t="str">
+      <c r="A18" s="68" t="str">
         <f aca="false">truthStateInitialUncertainty!A18</f>
         <v>sig_gyroy</v>
       </c>
-      <c r="B18" s="34" t="n">
+      <c r="B18" s="33" t="n">
         <f aca="false">truthStateInitialUncertainty!B18</f>
         <v>5</v>
       </c>
-      <c r="C18" s="34" t="str">
+      <c r="C18" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!C18</f>
         <v>deg/hr</v>
       </c>
-      <c r="D18" s="34" t="str">
+      <c r="D18" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!D18</f>
         <v>3-sigma initial gyro bias uncertainty</v>
       </c>
-      <c r="E18" s="79" t="n">
+      <c r="E18" s="78" t="n">
         <f aca="false">RADIANS(B18)/hr2sec/3</f>
         <v>8.08022801849227E-006</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="36" t="str">
+      <c r="A19" s="35" t="str">
         <f aca="false">truthStateInitialUncertainty!A19</f>
         <v>sig_gyroz</v>
       </c>
-      <c r="B19" s="38" t="n">
+      <c r="B19" s="37" t="n">
         <f aca="false">truthStateInitialUncertainty!B19</f>
         <v>5</v>
       </c>
-      <c r="C19" s="38" t="str">
+      <c r="C19" s="37" t="str">
         <f aca="false">truthStateInitialUncertainty!C19</f>
         <v>deg/hr</v>
       </c>
-      <c r="D19" s="38" t="str">
+      <c r="D19" s="37" t="str">
         <f aca="false">truthStateInitialUncertainty!D19</f>
         <v>3-sigma initial gyro bias uncertainty</v>
       </c>
-      <c r="E19" s="80" t="n">
+      <c r="E19" s="79" t="n">
         <f aca="false">RADIANS(B19)/hr2sec/3</f>
         <v>8.08022801849227E-006</v>
       </c>
@@ -3936,7 +3855,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M18" activeCellId="0" sqref="M18"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3949,309 +3868,309 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="65" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="78" t="s">
+      <c r="A1" s="64" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="67" t="s">
+      <c r="C1" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="67" t="s">
+      <c r="D1" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="68" t="s">
+      <c r="E1" s="67" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="69" t="s">
-        <v>164</v>
-      </c>
-      <c r="B2" s="34" t="n">
+      <c r="A2" s="68" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" s="33" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="79" t="n">
+      <c r="D2" s="33"/>
+      <c r="E2" s="78" t="n">
         <f aca="false">B2</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="69" t="s">
-        <v>165</v>
-      </c>
-      <c r="B3" s="34" t="n">
+      <c r="A3" s="68" t="s">
+        <v>154</v>
+      </c>
+      <c r="B3" s="33" t="n">
         <v>2</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="34"/>
-      <c r="E3" s="79" t="n">
+      <c r="D3" s="33"/>
+      <c r="E3" s="78" t="n">
         <f aca="false">B3</f>
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="69" t="s">
-        <v>166</v>
-      </c>
-      <c r="B4" s="34" t="n">
+      <c r="A4" s="68" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" s="33" t="n">
         <v>3</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="79" t="n">
+      <c r="D4" s="33"/>
+      <c r="E4" s="78" t="n">
         <f aca="false">B4</f>
         <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="69" t="s">
-        <v>167</v>
-      </c>
-      <c r="B5" s="34" t="n">
+      <c r="A5" s="68" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" s="33" t="n">
         <v>0.1</v>
       </c>
-      <c r="C5" s="34" t="str">
+      <c r="C5" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!C5</f>
         <v>m/sec</v>
       </c>
-      <c r="D5" s="34"/>
-      <c r="E5" s="79" t="n">
+      <c r="D5" s="33"/>
+      <c r="E5" s="78" t="n">
         <f aca="false">B5</f>
         <v>0.1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="69" t="s">
-        <v>168</v>
-      </c>
-      <c r="B6" s="34" t="n">
+      <c r="A6" s="68" t="s">
+        <v>157</v>
+      </c>
+      <c r="B6" s="33" t="n">
         <v>0.2</v>
       </c>
-      <c r="C6" s="34" t="str">
+      <c r="C6" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!C6</f>
         <v>m/sec</v>
       </c>
-      <c r="D6" s="34"/>
-      <c r="E6" s="79" t="n">
+      <c r="D6" s="33"/>
+      <c r="E6" s="78" t="n">
         <f aca="false">B6</f>
         <v>0.2</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="69" t="s">
-        <v>169</v>
-      </c>
-      <c r="B7" s="34" t="n">
+      <c r="A7" s="68" t="s">
+        <v>158</v>
+      </c>
+      <c r="B7" s="33" t="n">
         <v>0.3</v>
       </c>
-      <c r="C7" s="34" t="str">
+      <c r="C7" s="33" t="str">
         <f aca="false">truthStateInitialUncertainty!C7</f>
         <v>m/sec</v>
       </c>
-      <c r="D7" s="34"/>
-      <c r="E7" s="79" t="n">
+      <c r="D7" s="33"/>
+      <c r="E7" s="78" t="n">
         <f aca="false">B7</f>
         <v>0.3</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="69" t="s">
-        <v>170</v>
-      </c>
-      <c r="B8" s="34" t="n">
+      <c r="A8" s="68" t="s">
+        <v>159</v>
+      </c>
+      <c r="B8" s="33" t="n">
         <v>0.11</v>
       </c>
-      <c r="C8" s="34" t="s">
-        <v>171</v>
-      </c>
-      <c r="D8" s="34"/>
-      <c r="E8" s="79" t="n">
+      <c r="C8" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="D8" s="33"/>
+      <c r="E8" s="78" t="n">
         <f aca="false">RADIANS(B8)</f>
         <v>0.00191986217719376</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="69" t="s">
-        <v>172</v>
-      </c>
-      <c r="B9" s="34" t="n">
+      <c r="A9" s="68" t="s">
+        <v>161</v>
+      </c>
+      <c r="B9" s="33" t="n">
         <v>0.22</v>
       </c>
-      <c r="C9" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="D9" s="34"/>
-      <c r="E9" s="79" t="n">
+      <c r="C9" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="33"/>
+      <c r="E9" s="78" t="n">
         <f aca="false">RADIANS(B9)</f>
         <v>0.00383972435438752</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="69" t="s">
-        <v>173</v>
-      </c>
-      <c r="B10" s="34" t="n">
+      <c r="A10" s="68" t="s">
+        <v>162</v>
+      </c>
+      <c r="B10" s="33" t="n">
         <v>0.33</v>
       </c>
-      <c r="C10" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="D10" s="34"/>
-      <c r="E10" s="79" t="n">
+      <c r="C10" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="33"/>
+      <c r="E10" s="78" t="n">
         <f aca="false">RADIANS(B10)</f>
         <v>0.00575958653158129</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="69" t="s">
-        <v>174</v>
-      </c>
-      <c r="B11" s="34" t="n">
+      <c r="A11" s="68" t="s">
+        <v>163</v>
+      </c>
+      <c r="B11" s="33" t="n">
         <v>0.001</v>
       </c>
-      <c r="C11" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="34"/>
-      <c r="E11" s="79" t="n">
+      <c r="C11" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="33"/>
+      <c r="E11" s="78" t="n">
         <f aca="false">g2mps2*B11</f>
         <v>0.00981</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="69" t="s">
-        <v>175</v>
-      </c>
-      <c r="B12" s="34" t="n">
+      <c r="A12" s="68" t="s">
+        <v>164</v>
+      </c>
+      <c r="B12" s="33" t="n">
         <v>0.002</v>
       </c>
-      <c r="C12" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="D12" s="34"/>
-      <c r="E12" s="79" t="n">
+      <c r="C12" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="33"/>
+      <c r="E12" s="78" t="n">
         <f aca="false">g2mps2*B12</f>
         <v>0.01962</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="69" t="s">
-        <v>176</v>
-      </c>
-      <c r="B13" s="34" t="n">
+      <c r="A13" s="68" t="s">
+        <v>165</v>
+      </c>
+      <c r="B13" s="33" t="n">
         <v>0.003</v>
       </c>
-      <c r="C13" s="34" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="34"/>
-      <c r="E13" s="79" t="n">
+      <c r="C13" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="33"/>
+      <c r="E13" s="78" t="n">
         <f aca="false">g2mps2*B13</f>
         <v>0.02943</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="69" t="s">
-        <v>177</v>
-      </c>
-      <c r="B14" s="34" t="n">
+      <c r="A14" s="68" t="s">
+        <v>166</v>
+      </c>
+      <c r="B14" s="33" t="n">
         <v>1.1</v>
       </c>
-      <c r="C14" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="D14" s="34"/>
-      <c r="E14" s="79" t="n">
+      <c r="C14" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="33"/>
+      <c r="E14" s="78" t="n">
         <f aca="false">RADIANS(B14)/hr2sec</f>
         <v>5.3329504922049E-006</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="69" t="s">
-        <v>178</v>
-      </c>
-      <c r="B15" s="34" t="n">
+      <c r="A15" s="68" t="s">
+        <v>167</v>
+      </c>
+      <c r="B15" s="33" t="n">
         <v>1.2</v>
       </c>
-      <c r="C15" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="D15" s="34"/>
-      <c r="E15" s="79" t="n">
+      <c r="C15" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="33"/>
+      <c r="E15" s="78" t="n">
         <f aca="false">RADIANS(B15)/hr2sec</f>
         <v>5.81776417331443E-006</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="69" t="s">
-        <v>179</v>
-      </c>
-      <c r="B16" s="34" t="n">
+      <c r="A16" s="68" t="s">
+        <v>168</v>
+      </c>
+      <c r="B16" s="33" t="n">
         <v>1.3</v>
       </c>
-      <c r="C16" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="D16" s="34"/>
-      <c r="E16" s="79" t="n">
+      <c r="C16" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="33"/>
+      <c r="E16" s="78" t="n">
         <f aca="false">RADIANS(B16)/hr2sec</f>
         <v>6.30257785442397E-006</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="69" t="s">
-        <v>180</v>
-      </c>
-      <c r="B17" s="34" t="n">
+      <c r="A17" s="68" t="s">
+        <v>169</v>
+      </c>
+      <c r="B17" s="33" t="n">
         <v>0.01</v>
       </c>
-      <c r="C17" s="34" t="s">
+      <c r="C17" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="34"/>
-      <c r="E17" s="79" t="n">
+      <c r="D17" s="33"/>
+      <c r="E17" s="78" t="n">
         <f aca="false">B17</f>
         <v>0.01</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="69" t="s">
-        <v>181</v>
-      </c>
-      <c r="B18" s="34" t="n">
+      <c r="A18" s="68" t="s">
+        <v>170</v>
+      </c>
+      <c r="B18" s="33" t="n">
         <v>0.02</v>
       </c>
-      <c r="C18" s="34" t="s">
+      <c r="C18" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="34"/>
-      <c r="E18" s="79" t="n">
+      <c r="D18" s="33"/>
+      <c r="E18" s="78" t="n">
         <f aca="false">B18</f>
         <v>0.02</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="36" t="s">
-        <v>182</v>
-      </c>
-      <c r="B19" s="38" t="n">
+      <c r="A19" s="35" t="s">
+        <v>171</v>
+      </c>
+      <c r="B19" s="37" t="n">
         <v>0.03</v>
       </c>
-      <c r="C19" s="38" t="s">
+      <c r="C19" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="38"/>
-      <c r="E19" s="80" t="n">
+      <c r="D19" s="37"/>
+      <c r="E19" s="79" t="n">
         <f aca="false">B19</f>
         <v>0.03</v>
       </c>

</xml_diff>

<commit_message>
adding revisions from isaacs code
</commit_message>
<xml_diff>
--- a/config_randy.xlsx
+++ b/config_randy.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="189">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -170,21 +170,39 @@
     <t xml:space="preserve">r_body2antenna1_x</t>
   </si>
   <si>
+    <t xml:space="preserve">distance from body frame origin to antenna one, x dimension</t>
+  </si>
+  <si>
     <t xml:space="preserve">r_body2antenna1_y</t>
   </si>
   <si>
+    <t xml:space="preserve">distance from body frame origin to antenna one, y dimension</t>
+  </si>
+  <si>
     <t xml:space="preserve">r_body2antenna1_z</t>
   </si>
   <si>
+    <t xml:space="preserve">distance from body frame origin to antenna one, z dimension</t>
+  </si>
+  <si>
     <t xml:space="preserve">r_body2antenna2_x</t>
   </si>
   <si>
+    <t xml:space="preserve">distance from body frame origin to antenna two, x dimension</t>
+  </si>
+  <si>
     <t xml:space="preserve">r_body2antenna2_y</t>
   </si>
   <si>
+    <t xml:space="preserve">distance from body frame origin to antenna two, y dimension</t>
+  </si>
+  <si>
     <t xml:space="preserve">r_body2antenna2_z</t>
   </si>
   <si>
+    <t xml:space="preserve">distance from body frame origin to antenna two, z dimension</t>
+  </si>
+  <si>
     <t xml:space="preserve">nu</t>
   </si>
   <si>
@@ -500,6 +518,9 @@
     <t xml:space="preserve">del_rbix</t>
   </si>
   <si>
+    <t xml:space="preserve">Injected vehicle position error</t>
+  </si>
+  <si>
     <t xml:space="preserve">del_rbiy</t>
   </si>
   <si>
@@ -509,6 +530,9 @@
     <t xml:space="preserve">del_vbix</t>
   </si>
   <si>
+    <t xml:space="preserve">Injected vehicle velocity error</t>
+  </si>
+  <si>
     <t xml:space="preserve">del_vbiy</t>
   </si>
   <si>
@@ -521,6 +545,9 @@
     <t xml:space="preserve">deg </t>
   </si>
   <si>
+    <t xml:space="preserve">Injected vehicle quaternion error</t>
+  </si>
+  <si>
     <t xml:space="preserve">del_thy</t>
   </si>
   <si>
@@ -530,6 +557,9 @@
     <t xml:space="preserve">del_bax</t>
   </si>
   <si>
+    <t xml:space="preserve">Injected accel bias error</t>
+  </si>
+  <si>
     <t xml:space="preserve">del_bay</t>
   </si>
   <si>
@@ -539,6 +569,9 @@
     <t xml:space="preserve">del_bgx</t>
   </si>
   <si>
+    <t xml:space="preserve">Injected gyro bias error</t>
+  </si>
+  <si>
     <t xml:space="preserve">del_bgy</t>
   </si>
   <si>
@@ -546,6 +579,9 @@
   </si>
   <si>
     <t xml:space="preserve">del_rcix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Injected coil position error</t>
   </si>
   <si>
     <t xml:space="preserve">del_rciy</t>
@@ -582,7 +618,7 @@
     <numFmt numFmtId="169" formatCode="0.00E+00"/>
     <numFmt numFmtId="170" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -612,12 +648,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -745,7 +775,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="61">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -850,35 +880,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -890,7 +892,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -906,7 +908,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -918,23 +920,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -942,35 +928,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -986,14 +948,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1018,30 +972,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1063,6 +1001,22 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1145,13 +1099,13 @@
   </sheetPr>
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="75.57"/>
@@ -1345,7 +1299,7 @@
         <v>25</v>
       </c>
       <c r="B11" s="15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>13</v>
@@ -1355,7 +1309,7 @@
       </c>
       <c r="E11" s="14" t="n">
         <f aca="false">B11</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1477,7 +1431,7 @@
         <v>40</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>1</v>
+        <v>122000000</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>41</v>
@@ -1487,7 +1441,7 @@
       </c>
       <c r="E19" s="2" t="n">
         <f aca="false">B19</f>
-        <v>1</v>
+        <v>122000000</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1495,35 +1449,40 @@
         <v>43</v>
       </c>
       <c r="B20" s="1" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>34</v>
       </c>
+      <c r="D20" s="0" t="s">
+        <v>44</v>
+      </c>
       <c r="E20" s="2" t="n">
-        <f aca="false">B19</f>
-        <v>1</v>
+        <f aca="false">B20</f>
+        <v>0.5</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B21" s="1" t="n">
-        <f aca="false">1.5/4</f>
-        <v>0.375</v>
+        <v>1</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>34</v>
       </c>
+      <c r="D21" s="0" t="s">
+        <v>46</v>
+      </c>
       <c r="E21" s="2" t="n">
-        <f aca="false">B20</f>
-        <v>0</v>
+        <f aca="false">B21</f>
+        <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>0</v>
@@ -1531,45 +1490,53 @@
       <c r="C22" s="0" t="s">
         <v>34</v>
       </c>
+      <c r="D22" s="0" t="s">
+        <v>48</v>
+      </c>
       <c r="E22" s="2" t="n">
-        <f aca="false">B21</f>
-        <v>0.375</v>
+        <f aca="false">B22</f>
+        <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>34</v>
       </c>
+      <c r="D23" s="0" t="s">
+        <v>50</v>
+      </c>
       <c r="E23" s="2" t="n">
-        <f aca="false">B22</f>
-        <v>0</v>
+        <f aca="false">B23</f>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B24" s="1" t="n">
-        <f aca="false">-1.5/4</f>
-        <v>-0.375</v>
+        <v>1</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>34</v>
       </c>
+      <c r="D24" s="0" t="s">
+        <v>52</v>
+      </c>
       <c r="E24" s="2" t="n">
-        <f aca="false">B23</f>
-        <v>0</v>
+        <f aca="false">B24</f>
+        <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B25" s="1" t="n">
         <v>0</v>
@@ -1577,41 +1544,44 @@
       <c r="C25" s="0" t="s">
         <v>34</v>
       </c>
+      <c r="D25" s="0" t="s">
+        <v>54</v>
+      </c>
       <c r="E25" s="2" t="n">
-        <f aca="false">B24</f>
-        <v>-0.375</v>
+        <f aca="false">B25</f>
+        <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="B26" s="1" t="n">
         <v>0</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E26" s="2" t="n">
-        <f aca="false">B25</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <f aca="false">B26</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B27" s="1" t="n">
         <v>3335640000</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="E27" s="2" t="n">
         <f aca="false">B27</f>
@@ -1649,7 +1619,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
       <c r="B1" s="0" t="n">
         <v>60</v>
@@ -1657,7 +1627,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>60</v>
@@ -1665,7 +1635,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>174</v>
+        <v>186</v>
       </c>
       <c r="B3" s="0" t="n">
         <f aca="false">hr2min*min2sec</f>
@@ -1674,7 +1644,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>9.81</v>
@@ -1682,7 +1652,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>24</v>
@@ -1706,8 +1676,8 @@
   </sheetPr>
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1721,270 +1691,270 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="27" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="31" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" s="32" t="s">
+      <c r="A2" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" s="34" t="n">
+      <c r="D2" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="27" t="n">
         <f aca="false">B2</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" s="37" t="s">
+      <c r="A3" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="E3" s="38" t="n">
+      <c r="D3" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="31" t="n">
         <f aca="false">B3</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="33" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="40" t="n">
-        <v>10</v>
-      </c>
-      <c r="C4" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="41" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="42" t="n">
+      <c r="D4" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="35" t="n">
         <f aca="false">B4</f>
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="43" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" s="40" t="n">
-        <v>22.5</v>
-      </c>
-      <c r="C5" s="44" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="41" t="s">
-        <v>63</v>
-      </c>
-      <c r="E5" s="42" t="n">
+      <c r="A5" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="33" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="35" t="n">
         <f aca="false">RADIANS(B5)</f>
-        <v>0.392699081698724</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="43" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6" s="40" t="n">
-        <v>-3</v>
-      </c>
-      <c r="C6" s="44" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6" s="41" t="s">
-        <v>65</v>
-      </c>
-      <c r="E6" s="42" t="n">
+      <c r="A6" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="33" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="35" t="n">
         <f aca="false">RADIANS(B6)</f>
-        <v>-0.0523598775598299</v>
+        <v>0.0872664625997165</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="45" t="s">
-        <v>66</v>
-      </c>
-      <c r="B7" s="31" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" s="32" t="s">
+      <c r="A7" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" s="26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="E7" s="34" t="n">
+      <c r="D7" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="27" t="n">
         <f aca="false">B7*g2mps2</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="46" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="47" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" s="33" t="s">
+      <c r="A8" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="E8" s="48" t="n">
+      <c r="D8" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="37" t="n">
         <f aca="false">B8*g2mps2</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="49" t="s">
-        <v>70</v>
-      </c>
-      <c r="B9" s="50" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" s="37" t="s">
+      <c r="A9" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="38" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="E9" s="38" t="n">
+      <c r="D9" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="31" t="n">
         <f aca="false">B9*g2mps2</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="51" t="s">
-        <v>72</v>
-      </c>
-      <c r="B10" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="C10" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="D10" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="E10" s="53" t="n">
+      <c r="A10" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="39" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="10" t="n">
         <f aca="false">RADIANS(B10)/hr2sec</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="51" t="s">
-        <v>75</v>
-      </c>
-      <c r="B11" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="D11" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="E11" s="55" t="n">
+      <c r="A11" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" s="14" t="n">
         <f aca="false">RADIANS(B11)/hr2sec</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="51" t="s">
-        <v>77</v>
-      </c>
-      <c r="B12" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" s="37" t="s">
-        <v>73</v>
-      </c>
-      <c r="D12" s="33" t="s">
-        <v>78</v>
-      </c>
-      <c r="E12" s="57" t="n">
+      <c r="A12" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="38" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" s="40" t="n">
         <f aca="false">RADIANS(B12)/hr2sec</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="B13" s="52" t="n">
+        <v>85</v>
+      </c>
+      <c r="B13" s="39" t="n">
         <v>0</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="E13" s="58" t="n">
+      <c r="D13" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" s="41" t="n">
         <f aca="false">B13</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="B14" s="54" t="n">
+        <v>87</v>
+      </c>
+      <c r="B14" s="36" t="n">
         <v>0</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="33" t="s">
-        <v>82</v>
-      </c>
-      <c r="E14" s="59" t="n">
+      <c r="D14" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E14" s="42" t="n">
         <f aca="false">B14</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="B15" s="56" t="n">
-        <v>0</v>
-      </c>
-      <c r="C15" s="61" t="s">
+      <c r="A15" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="38" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="E15" s="62" t="n">
+      <c r="D15" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="E15" s="43" t="n">
         <f aca="false">B15</f>
         <v>0</v>
       </c>
@@ -2022,24 +1992,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
@@ -2056,7 +2026,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>3</v>
@@ -2073,7 +2043,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>4</v>
@@ -2090,7 +2060,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>5</v>
@@ -2106,8 +2076,8 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="45" t="s">
-        <v>92</v>
+      <c r="A6" s="7" t="s">
+        <v>98</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>6</v>
@@ -2124,7 +2094,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>9</v>
@@ -2141,7 +2111,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>12</v>
@@ -2158,7 +2128,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>1</v>
@@ -2175,7 +2145,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>6</v>
@@ -2223,24 +2193,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
@@ -2257,7 +2227,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>4</v>
@@ -2274,7 +2244,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>7</v>
@@ -2291,7 +2261,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>11</v>
@@ -2308,7 +2278,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>14</v>
@@ -2325,7 +2295,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>17</v>
@@ -2342,7 +2312,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B8" s="0" t="n">
         <f aca="false">B2</f>
@@ -2361,7 +2331,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B9" s="0" t="n">
         <f aca="false">B5</f>
@@ -2404,7 +2374,7 @@
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="63" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="44" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="48.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="14.71"/>
@@ -2413,216 +2383,216 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="65" t="s">
+      <c r="A1" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="67" t="s">
+      <c r="E1" s="48" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="68" t="s">
-        <v>98</v>
-      </c>
-      <c r="B2" s="69" t="n">
+      <c r="A2" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="49" t="n">
         <f aca="false">0.00000016*3</f>
         <v>4.8E-007</v>
       </c>
-      <c r="C2" s="33" t="s">
-        <v>99</v>
+      <c r="C2" s="13" t="s">
+        <v>105</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="E2" s="55" t="n">
+        <v>106</v>
+      </c>
+      <c r="E2" s="14" t="n">
         <f aca="false">B2/3</f>
         <v>1.6E-007</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="68" t="s">
-        <v>101</v>
-      </c>
-      <c r="B3" s="70" t="n">
+      <c r="A3" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="C3" s="69" t="s">
-        <v>73</v>
-      </c>
-      <c r="D3" s="33" t="s">
-        <v>102</v>
-      </c>
-      <c r="E3" s="55" t="n">
+      <c r="C3" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E3" s="14" t="n">
         <f aca="false">RADIANS(B3)/hr2sec/3</f>
         <v>8.08022801849227E-006</v>
       </c>
       <c r="F3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="35" t="s">
-        <v>103</v>
-      </c>
-      <c r="B4" s="71" t="n">
+      <c r="A4" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="50" t="n">
         <v>0.05</v>
       </c>
-      <c r="C4" s="37" t="s">
-        <v>104</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>105</v>
-      </c>
-      <c r="E4" s="57" t="n">
+      <c r="C4" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4" s="40" t="n">
         <f aca="false">RADIANS(B4)/SQRT(hr2sec)/3</f>
         <v>4.84813681109536E-006</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="68" t="s">
-        <v>106</v>
-      </c>
-      <c r="B5" s="70" t="n">
+      <c r="A5" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="16" t="n">
         <v>20</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="E5" s="55" t="n">
+        <v>114</v>
+      </c>
+      <c r="E5" s="14" t="n">
         <f aca="false">RADIANS(B5)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="68" t="s">
-        <v>109</v>
-      </c>
-      <c r="B6" s="70" t="n">
+      <c r="A6" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" s="16" t="n">
         <v>20</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="E6" s="55" t="n">
+        <v>116</v>
+      </c>
+      <c r="E6" s="14" t="n">
         <f aca="false">RADIANS(B6)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="B7" s="70" t="n">
+        <v>117</v>
+      </c>
+      <c r="B7" s="16" t="n">
         <v>1.5</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="E7" s="55" t="n">
+        <v>119</v>
+      </c>
+      <c r="E7" s="14" t="n">
         <f aca="false">RADIANS(B7)/3600/3</f>
         <v>2.42406840554768E-006</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="B8" s="70" t="n">
+        <v>120</v>
+      </c>
+      <c r="B8" s="16" t="n">
         <v>1.5</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="E8" s="55" t="n">
+        <v>119</v>
+      </c>
+      <c r="E8" s="14" t="n">
         <f aca="false">RADIANS(B8)/3600/3</f>
         <v>2.42406840554768E-006</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="B9" s="70" t="n">
+        <v>121</v>
+      </c>
+      <c r="B9" s="16" t="n">
         <v>9</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="E9" s="55" t="n">
+        <v>119</v>
+      </c>
+      <c r="E9" s="14" t="n">
         <f aca="false">RADIANS(B9)/3600/3</f>
         <v>1.45444104332861E-005</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B10" s="72" t="n">
+        <v>122</v>
+      </c>
+      <c r="B10" s="26" t="n">
         <v>3</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="E10" s="53" t="n">
+        <v>124</v>
+      </c>
+      <c r="E10" s="10" t="n">
         <f aca="false">B10/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="60" t="s">
-        <v>119</v>
-      </c>
-      <c r="B11" s="73" t="n">
+      <c r="A11" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" s="29" t="n">
         <v>3</v>
       </c>
-      <c r="C11" s="61" t="s">
-        <v>117</v>
-      </c>
-      <c r="D11" s="61" t="s">
-        <v>120</v>
-      </c>
-      <c r="E11" s="57" t="n">
+      <c r="C11" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="E11" s="40" t="n">
         <f aca="false">B11/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="B12" s="63" t="n">
+        <v>127</v>
+      </c>
+      <c r="B12" s="44" t="n">
         <v>10</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>34</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="E12" s="2" t="n">
         <f aca="false">B12/3</f>
@@ -2631,16 +2601,16 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="B13" s="63" t="n">
+        <v>129</v>
+      </c>
+      <c r="B13" s="44" t="n">
         <v>100</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>34</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="E13" s="2" t="n">
         <f aca="false">B13/3</f>
@@ -2649,16 +2619,16 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="B14" s="63" t="n">
+        <v>131</v>
+      </c>
+      <c r="B14" s="44" t="n">
         <v>10</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>34</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="E14" s="2" t="n">
         <f aca="false">B14/3</f>
@@ -2689,360 +2659,360 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="9.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="33" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="33" width="51.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="74" width="14.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="33" width="17.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="33" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="9.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="13" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="13" width="51.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="51" width="14.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="13" width="17.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="13" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="27" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="B2" s="32" t="n">
+      <c r="A2" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" s="9" t="n">
         <v>4000</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="32" t="s">
-        <v>128</v>
-      </c>
-      <c r="E2" s="53" t="n">
+      <c r="D2" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" s="10" t="n">
         <f aca="false">B2/3</f>
         <v>1333.33333333333</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="68" t="s">
-        <v>129</v>
-      </c>
-      <c r="B3" s="33" t="n">
+      <c r="A3" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" s="13" t="n">
         <v>4000</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="33" t="s">
-        <v>128</v>
-      </c>
-      <c r="E3" s="55" t="n">
+      <c r="D3" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E3" s="14" t="n">
         <f aca="false">B3/3</f>
         <v>1333.33333333333</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="68" t="s">
-        <v>130</v>
-      </c>
-      <c r="B4" s="33" t="n">
+      <c r="A4" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4" s="13" t="n">
         <v>4000</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="33" t="s">
-        <v>128</v>
-      </c>
-      <c r="E4" s="55" t="n">
+      <c r="D4" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E4" s="14" t="n">
         <f aca="false">B4/3</f>
         <v>1333.33333333333</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="68" t="s">
-        <v>131</v>
-      </c>
-      <c r="B5" s="33" t="n">
+      <c r="A5" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="C5" s="33" t="s">
-        <v>132</v>
-      </c>
-      <c r="D5" s="33" t="s">
-        <v>133</v>
-      </c>
-      <c r="E5" s="55" t="n">
+      <c r="C5" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="E5" s="14" t="n">
         <f aca="false">B5/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="68" t="s">
-        <v>134</v>
-      </c>
-      <c r="B6" s="33" t="n">
+      <c r="A6" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="C6" s="33" t="s">
-        <v>132</v>
-      </c>
-      <c r="D6" s="33" t="s">
-        <v>133</v>
-      </c>
-      <c r="E6" s="55" t="n">
+      <c r="C6" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="E6" s="14" t="n">
         <f aca="false">B6/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="68" t="s">
-        <v>135</v>
-      </c>
-      <c r="B7" s="33" t="n">
+      <c r="A7" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B7" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="C7" s="33" t="s">
-        <v>132</v>
-      </c>
-      <c r="D7" s="33" t="s">
-        <v>133</v>
-      </c>
-      <c r="E7" s="55" t="n">
+      <c r="C7" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="E7" s="14" t="n">
         <f aca="false">B7/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="68" t="s">
-        <v>136</v>
-      </c>
-      <c r="B8" s="33" t="n">
+      <c r="A8" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" s="13" t="n">
         <v>0.0005</v>
       </c>
-      <c r="C8" s="33" t="s">
-        <v>137</v>
-      </c>
-      <c r="D8" s="33" t="s">
-        <v>138</v>
-      </c>
-      <c r="E8" s="55" t="n">
+      <c r="C8" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E8" s="14" t="n">
         <f aca="false">B8/3</f>
         <v>0.000166666666666667</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="68" t="s">
-        <v>139</v>
-      </c>
-      <c r="B9" s="33" t="n">
+      <c r="A9" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B9" s="13" t="n">
         <v>0.0005</v>
       </c>
-      <c r="C9" s="33" t="s">
-        <v>137</v>
-      </c>
-      <c r="D9" s="33" t="s">
-        <v>138</v>
-      </c>
-      <c r="E9" s="55" t="n">
+      <c r="C9" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E9" s="14" t="n">
         <f aca="false">B9/3</f>
         <v>0.000166666666666667</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="68" t="s">
-        <v>140</v>
-      </c>
-      <c r="B10" s="33" t="n">
+      <c r="A10" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="B10" s="13" t="n">
         <v>0.0005</v>
       </c>
-      <c r="C10" s="33" t="s">
-        <v>137</v>
-      </c>
-      <c r="D10" s="33" t="s">
-        <v>138</v>
-      </c>
-      <c r="E10" s="55" t="n">
+      <c r="C10" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E10" s="14" t="n">
         <f aca="false">B10/3</f>
         <v>0.000166666666666667</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="68" t="s">
-        <v>141</v>
-      </c>
-      <c r="B11" s="33" t="n">
+      <c r="A11" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="B11" s="13" t="n">
         <f aca="false">truthStateParams!$B$5</f>
         <v>20</v>
       </c>
-      <c r="C11" s="33" t="s">
-        <v>112</v>
+      <c r="C11" s="13" t="s">
+        <v>118</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="E11" s="55" t="n">
+        <v>148</v>
+      </c>
+      <c r="E11" s="14" t="n">
         <f aca="false">RADIANS(B11)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="B12" s="33" t="n">
+        <v>149</v>
+      </c>
+      <c r="B12" s="13" t="n">
         <f aca="false">truthStateParams!$B$5</f>
         <v>20</v>
       </c>
-      <c r="C12" s="33" t="s">
-        <v>112</v>
+      <c r="C12" s="13" t="s">
+        <v>118</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="E12" s="55" t="n">
+        <v>148</v>
+      </c>
+      <c r="E12" s="14" t="n">
         <f aca="false">RADIANS(B12)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="B13" s="33" t="n">
+        <v>150</v>
+      </c>
+      <c r="B13" s="13" t="n">
         <f aca="false">truthStateParams!$B$5</f>
         <v>20</v>
       </c>
-      <c r="C13" s="33" t="s">
-        <v>112</v>
+      <c r="C13" s="13" t="s">
+        <v>118</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="E13" s="55" t="n">
+        <v>148</v>
+      </c>
+      <c r="E13" s="14" t="n">
         <f aca="false">RADIANS(B13)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="B14" s="33" t="n">
+        <v>151</v>
+      </c>
+      <c r="B14" s="13" t="n">
         <f aca="false">truthStateParams!$B$6</f>
         <v>20</v>
       </c>
-      <c r="C14" s="33" t="s">
-        <v>112</v>
+      <c r="C14" s="13" t="s">
+        <v>118</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="E14" s="55" t="n">
+        <v>152</v>
+      </c>
+      <c r="E14" s="14" t="n">
         <f aca="false">RADIANS(B14)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="B15" s="33" t="n">
+        <v>153</v>
+      </c>
+      <c r="B15" s="13" t="n">
         <f aca="false">truthStateParams!$B$6</f>
         <v>20</v>
       </c>
-      <c r="C15" s="33" t="s">
-        <v>112</v>
+      <c r="C15" s="13" t="s">
+        <v>118</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="E15" s="55" t="n">
+        <v>152</v>
+      </c>
+      <c r="E15" s="14" t="n">
         <f aca="false">RADIANS(B15)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="B16" s="33" t="n">
+        <v>154</v>
+      </c>
+      <c r="B16" s="13" t="n">
         <f aca="false">truthStateParams!$B$6</f>
         <v>20</v>
       </c>
-      <c r="C16" s="33" t="s">
-        <v>112</v>
+      <c r="C16" s="13" t="s">
+        <v>118</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="E16" s="55" t="n">
+        <v>152</v>
+      </c>
+      <c r="E16" s="14" t="n">
         <f aca="false">RADIANS(B16)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="68" t="s">
-        <v>149</v>
-      </c>
-      <c r="B17" s="33" t="n">
+      <c r="A17" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="B17" s="13" t="n">
         <f aca="false">truthStateParams!$B$3</f>
         <v>5</v>
       </c>
-      <c r="C17" s="69" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17" s="33" t="s">
-        <v>150</v>
-      </c>
-      <c r="E17" s="55" t="n">
+      <c r="C17" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="E17" s="14" t="n">
         <f aca="false">RADIANS(B17)/hr2sec/3</f>
         <v>8.08022801849227E-006</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="68" t="s">
-        <v>151</v>
-      </c>
-      <c r="B18" s="33" t="n">
+      <c r="A18" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="B18" s="13" t="n">
         <f aca="false">truthStateParams!$B$3</f>
         <v>5</v>
       </c>
-      <c r="C18" s="69" t="s">
-        <v>73</v>
-      </c>
-      <c r="D18" s="33" t="s">
-        <v>150</v>
-      </c>
-      <c r="E18" s="55" t="n">
+      <c r="C18" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="E18" s="14" t="n">
         <f aca="false">RADIANS(B18)/hr2sec/3</f>
         <v>8.08022801849227E-006</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="35" t="s">
-        <v>152</v>
-      </c>
-      <c r="B19" s="37" t="n">
+      <c r="A19" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="B19" s="30" t="n">
         <f aca="false">truthStateParams!$B$3</f>
         <v>5</v>
       </c>
-      <c r="C19" s="75" t="s">
-        <v>73</v>
-      </c>
-      <c r="D19" s="37" t="s">
-        <v>150</v>
-      </c>
-      <c r="E19" s="57" t="n">
+      <c r="C19" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="E19" s="40" t="n">
         <f aca="false">RADIANS(B19)/hr2sec/3</f>
         <v>8.08022801849227E-006</v>
       </c>
@@ -3071,42 +3041,42 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="76" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="33" width="11.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="33" width="46.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="74" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="33" width="25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="33" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="53" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="13" width="11.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="13" width="46.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="51" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="13" width="25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="13" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="65" t="s">
+      <c r="A1" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="67" t="s">
+      <c r="E1" s="48" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="68" t="str">
+      <c r="A2" s="11" t="str">
         <f aca="false">truthStateParams!A2</f>
         <v>Q_grav</v>
       </c>
-      <c r="B2" s="69" t="n">
+      <c r="B2" s="49" t="n">
         <f aca="false">truthStateParams!B2</f>
         <v>4.8E-007</v>
       </c>
-      <c r="C2" s="33" t="str">
+      <c r="C2" s="13" t="str">
         <f aca="false">truthStateParams!C2</f>
         <v>m^2/s^3</v>
       </c>
@@ -3114,64 +3084,64 @@
         <f aca="false">truthStateParams!D2</f>
         <v>3-sigma non-gravitational process noise</v>
       </c>
-      <c r="E2" s="55" t="n">
+      <c r="E2" s="14" t="n">
         <f aca="false">B2/3</f>
         <v>1.6E-007</v>
       </c>
-      <c r="F2" s="74"/>
+      <c r="F2" s="51"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="68" t="str">
+      <c r="A3" s="11" t="str">
         <f aca="false">truthStateParams!A3</f>
         <v>sig_gyro_ss</v>
       </c>
-      <c r="B3" s="70" t="n">
+      <c r="B3" s="16" t="n">
         <f aca="false">truthStateParams!B3</f>
         <v>5</v>
       </c>
-      <c r="C3" s="69" t="str">
+      <c r="C3" s="49" t="str">
         <f aca="false">truthStateParams!C3</f>
         <v>deg/hr</v>
       </c>
-      <c r="D3" s="33" t="str">
+      <c r="D3" s="13" t="str">
         <f aca="false">truthStateParams!D3</f>
         <v>3-sigma steady-state gyro bias</v>
       </c>
-      <c r="E3" s="55" t="n">
+      <c r="E3" s="14" t="n">
         <f aca="false">RADIANS(B3)/hr2sec/3</f>
         <v>8.08022801849227E-006</v>
       </c>
-      <c r="F3" s="74"/>
+      <c r="F3" s="51"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="35" t="str">
+      <c r="A4" s="28" t="str">
         <f aca="false">truthStateParams!A4</f>
         <v>arw</v>
       </c>
-      <c r="B4" s="71" t="n">
+      <c r="B4" s="50" t="n">
         <f aca="false">truthStateParams!B4</f>
         <v>0.05</v>
       </c>
-      <c r="C4" s="37" t="str">
+      <c r="C4" s="30" t="str">
         <f aca="false">truthStateParams!C4</f>
         <v>deg/sqrt(hr)</v>
       </c>
-      <c r="D4" s="37" t="str">
+      <c r="D4" s="30" t="str">
         <f aca="false">truthStateParams!D4</f>
         <v>3-sigma angular random walk</v>
       </c>
-      <c r="E4" s="57" t="n">
+      <c r="E4" s="40" t="n">
         <f aca="false">RADIANS(B4)/SQRT(hr2sec)/3</f>
         <v>4.84813681109536E-006</v>
       </c>
-      <c r="F4" s="74"/>
+      <c r="F4" s="51"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="68" t="str">
+      <c r="A5" s="11" t="str">
         <f aca="false">truthStateParams!A5</f>
         <v>sig_st_ss</v>
       </c>
-      <c r="B5" s="70" t="n">
+      <c r="B5" s="16" t="n">
         <f aca="false">truthStateParams!B5</f>
         <v>20</v>
       </c>
@@ -3183,18 +3153,18 @@
         <f aca="false">truthStateParams!D5</f>
         <v>3-sigma steady-state star camera misalignment</v>
       </c>
-      <c r="E5" s="55" t="n">
+      <c r="E5" s="14" t="n">
         <f aca="false">RADIANS(B5)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
-      <c r="F5" s="74"/>
+      <c r="F5" s="51"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="68" t="str">
+      <c r="A6" s="11" t="str">
         <f aca="false">truthStateParams!A6</f>
         <v>sig_c_ss</v>
       </c>
-      <c r="B6" s="70" t="n">
+      <c r="B6" s="16" t="n">
         <f aca="false">truthStateParams!B6</f>
         <v>20</v>
       </c>
@@ -3206,7 +3176,7 @@
         <f aca="false">truthStateParams!D6</f>
         <v>3-sigma steady-state terrain camera misalignment</v>
       </c>
-      <c r="E6" s="55" t="n">
+      <c r="E6" s="14" t="n">
         <f aca="false">RADIANS(B6)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
@@ -3216,7 +3186,7 @@
         <f aca="false">truthStateParams!A7</f>
         <v>sig_meas_stx</v>
       </c>
-      <c r="B7" s="70" t="n">
+      <c r="B7" s="16" t="n">
         <f aca="false">truthStateParams!B7</f>
         <v>1.5</v>
       </c>
@@ -3228,7 +3198,7 @@
         <f aca="false">truthStateParams!D7</f>
         <v>3-sigma star camera measurement uncertainty</v>
       </c>
-      <c r="E7" s="55" t="n">
+      <c r="E7" s="14" t="n">
         <f aca="false">RADIANS(B7)/3600/3</f>
         <v>2.42406840554768E-006</v>
       </c>
@@ -3238,7 +3208,7 @@
         <f aca="false">truthStateParams!A8</f>
         <v>sig_meas_sty</v>
       </c>
-      <c r="B8" s="70" t="n">
+      <c r="B8" s="16" t="n">
         <f aca="false">truthStateParams!B8</f>
         <v>1.5</v>
       </c>
@@ -3250,7 +3220,7 @@
         <f aca="false">truthStateParams!D8</f>
         <v>3-sigma star camera measurement uncertainty</v>
       </c>
-      <c r="E8" s="55" t="n">
+      <c r="E8" s="14" t="n">
         <f aca="false">RADIANS(B8)/3600/3</f>
         <v>2.42406840554768E-006</v>
       </c>
@@ -3260,7 +3230,7 @@
         <f aca="false">truthStateParams!A9</f>
         <v>sig_meas_stz</v>
       </c>
-      <c r="B9" s="70" t="n">
+      <c r="B9" s="16" t="n">
         <f aca="false">truthStateParams!B9</f>
         <v>9</v>
       </c>
@@ -3272,7 +3242,7 @@
         <f aca="false">truthStateParams!D9</f>
         <v>3-sigma star camera measurement uncertainty</v>
       </c>
-      <c r="E9" s="55" t="n">
+      <c r="E9" s="14" t="n">
         <f aca="false">RADIANS(B9)/3600/3</f>
         <v>1.45444104332861E-005</v>
       </c>
@@ -3282,7 +3252,7 @@
         <f aca="false">truthStateParams!A10</f>
         <v>sig_cu</v>
       </c>
-      <c r="B10" s="72" t="n">
+      <c r="B10" s="26" t="n">
         <f aca="false">truthStateParams!B10</f>
         <v>3</v>
       </c>
@@ -3294,95 +3264,95 @@
         <f aca="false">truthStateParams!D10</f>
         <v>3-sigma u component of pixel noise</v>
       </c>
-      <c r="E10" s="53" t="n">
+      <c r="E10" s="10" t="n">
         <f aca="false">B10/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="60" t="str">
+      <c r="A11" s="28" t="str">
         <f aca="false">truthStateParams!A11</f>
         <v>sig_cv</v>
       </c>
-      <c r="B11" s="73" t="n">
+      <c r="B11" s="29" t="n">
         <f aca="false">truthStateParams!B11</f>
         <v>3</v>
       </c>
-      <c r="C11" s="61" t="str">
+      <c r="C11" s="30" t="str">
         <f aca="false">truthStateParams!C11</f>
         <v>pixels</v>
       </c>
-      <c r="D11" s="61" t="str">
+      <c r="D11" s="30" t="str">
         <f aca="false">truthStateParams!D11</f>
         <v>3-sigma v component of pixel noise</v>
       </c>
-      <c r="E11" s="57" t="n">
+      <c r="E11" s="40" t="n">
         <f aca="false">B11/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="60" t="str">
+      <c r="A12" s="28" t="str">
         <f aca="false">truthStateParams!A12</f>
         <v>sig_idpos</v>
       </c>
-      <c r="B12" s="73" t="n">
+      <c r="B12" s="29" t="n">
         <f aca="false">truthStateParams!B12</f>
         <v>10</v>
       </c>
-      <c r="C12" s="61" t="str">
+      <c r="C12" s="30" t="str">
         <f aca="false">truthStateParams!C12</f>
         <v>m</v>
       </c>
-      <c r="D12" s="61" t="str">
+      <c r="D12" s="30" t="str">
         <f aca="false">truthStateParams!D12</f>
         <v>3-sigma change in inertial position measurement uncertainty</v>
       </c>
-      <c r="E12" s="57" t="n">
+      <c r="E12" s="40" t="n">
         <f aca="false">B12/3</f>
         <v>3.33333333333333</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="60" t="str">
+      <c r="A13" s="28" t="str">
         <f aca="false">truthStateParams!A13</f>
         <v>sig_loss</v>
       </c>
-      <c r="B13" s="73" t="n">
+      <c r="B13" s="29" t="n">
         <f aca="false">truthStateParams!B13</f>
         <v>100</v>
       </c>
-      <c r="C13" s="61" t="str">
+      <c r="C13" s="30" t="str">
         <f aca="false">truthStateParams!C13</f>
         <v>m</v>
       </c>
-      <c r="D13" s="61" t="str">
+      <c r="D13" s="30" t="str">
         <f aca="false">truthStateParams!D13</f>
         <v>3-sigma LOSS feature location uncertainty</v>
       </c>
-      <c r="E13" s="57" t="n">
+      <c r="E13" s="40" t="n">
         <f aca="false">B13/3</f>
         <v>33.3333333333333</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="60" t="str">
+      <c r="A14" s="28" t="str">
         <f aca="false">truthStateParams!A14</f>
         <v>sig_mdpos</v>
       </c>
-      <c r="B14" s="73" t="n">
+      <c r="B14" s="29" t="n">
         <f aca="false">truthStateParams!B14</f>
         <v>10</v>
       </c>
-      <c r="C14" s="61" t="str">
+      <c r="C14" s="30" t="str">
         <f aca="false">truthStateParams!C14</f>
         <v>m</v>
       </c>
-      <c r="D14" s="61" t="str">
+      <c r="D14" s="30" t="str">
         <f aca="false">truthStateParams!D14</f>
         <v>3-sigma change in lunar-referenced position measurement uncertainty</v>
       </c>
-      <c r="E14" s="57" t="n">
+      <c r="E14" s="40" t="n">
         <f aca="false">B14/3</f>
         <v>3.33333333333333</v>
       </c>
@@ -3411,427 +3381,427 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="9.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="33" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="33" width="51.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="74" width="13.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="33" width="14.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="33" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="13" width="9.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="13" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="13" width="51.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="51" width="13.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="13" width="14.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="13" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="77" t="s">
+      <c r="A1" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="68" t="str">
+      <c r="A2" s="11" t="str">
         <f aca="false">truthStateInitialUncertainty!A2</f>
         <v>sig_rsx</v>
       </c>
-      <c r="B2" s="33" t="n">
+      <c r="B2" s="13" t="n">
         <f aca="false">truthStateInitialUncertainty!B2</f>
         <v>4000</v>
       </c>
-      <c r="C2" s="33" t="str">
+      <c r="C2" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!C2</f>
         <v>m</v>
       </c>
-      <c r="D2" s="33" t="str">
+      <c r="D2" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!D2</f>
         <v>3-sigma initial satellite position uncertainty</v>
       </c>
-      <c r="E2" s="78" t="n">
+      <c r="E2" s="55" t="n">
         <f aca="false">B2/3</f>
         <v>1333.33333333333</v>
       </c>
-      <c r="F2" s="74"/>
+      <c r="F2" s="51"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="68" t="str">
+      <c r="A3" s="11" t="str">
         <f aca="false">truthStateInitialUncertainty!A3</f>
         <v>sig_rsy</v>
       </c>
-      <c r="B3" s="33" t="n">
+      <c r="B3" s="13" t="n">
         <f aca="false">truthStateInitialUncertainty!B3</f>
         <v>4000</v>
       </c>
-      <c r="C3" s="33" t="str">
+      <c r="C3" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!C3</f>
         <v>m</v>
       </c>
-      <c r="D3" s="33" t="str">
+      <c r="D3" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!D3</f>
         <v>3-sigma initial satellite position uncertainty</v>
       </c>
-      <c r="E3" s="78" t="n">
+      <c r="E3" s="55" t="n">
         <f aca="false">B3/3</f>
         <v>1333.33333333333</v>
       </c>
-      <c r="F3" s="74"/>
+      <c r="F3" s="51"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="68" t="str">
+      <c r="A4" s="11" t="str">
         <f aca="false">truthStateInitialUncertainty!A4</f>
         <v>sig_rsz</v>
       </c>
-      <c r="B4" s="33" t="n">
+      <c r="B4" s="13" t="n">
         <f aca="false">truthStateInitialUncertainty!B4</f>
         <v>4000</v>
       </c>
-      <c r="C4" s="33" t="str">
+      <c r="C4" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!C4</f>
         <v>m</v>
       </c>
-      <c r="D4" s="33" t="str">
+      <c r="D4" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!D4</f>
         <v>3-sigma initial satellite position uncertainty</v>
       </c>
-      <c r="E4" s="78" t="n">
+      <c r="E4" s="55" t="n">
         <f aca="false">B4/3</f>
         <v>1333.33333333333</v>
       </c>
-      <c r="F4" s="74"/>
+      <c r="F4" s="51"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="68" t="str">
+      <c r="A5" s="11" t="str">
         <f aca="false">truthStateInitialUncertainty!A5</f>
         <v>sig_vsx</v>
       </c>
-      <c r="B5" s="33" t="n">
+      <c r="B5" s="13" t="n">
         <f aca="false">truthStateInitialUncertainty!B5</f>
         <v>3</v>
       </c>
-      <c r="C5" s="33" t="str">
+      <c r="C5" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!C5</f>
         <v>m/sec</v>
       </c>
-      <c r="D5" s="33" t="str">
+      <c r="D5" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!D5</f>
         <v>3-sigma initial satellite velocity uncertainty</v>
       </c>
-      <c r="E5" s="78" t="n">
+      <c r="E5" s="55" t="n">
         <f aca="false">B5/3</f>
         <v>1</v>
       </c>
-      <c r="F5" s="74"/>
+      <c r="F5" s="51"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="68" t="str">
+      <c r="A6" s="11" t="str">
         <f aca="false">truthStateInitialUncertainty!A6</f>
         <v>sig_vsy</v>
       </c>
-      <c r="B6" s="33" t="n">
+      <c r="B6" s="13" t="n">
         <f aca="false">truthStateInitialUncertainty!B6</f>
         <v>3</v>
       </c>
-      <c r="C6" s="33" t="str">
+      <c r="C6" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!C6</f>
         <v>m/sec</v>
       </c>
-      <c r="D6" s="33" t="str">
+      <c r="D6" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!D6</f>
         <v>3-sigma initial satellite velocity uncertainty</v>
       </c>
-      <c r="E6" s="78" t="n">
+      <c r="E6" s="55" t="n">
         <f aca="false">B6/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="68" t="str">
+      <c r="A7" s="11" t="str">
         <f aca="false">truthStateInitialUncertainty!A7</f>
         <v>sig_vsz</v>
       </c>
-      <c r="B7" s="33" t="n">
+      <c r="B7" s="13" t="n">
         <f aca="false">truthStateInitialUncertainty!B7</f>
         <v>3</v>
       </c>
-      <c r="C7" s="33" t="str">
+      <c r="C7" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!C7</f>
         <v>m/sec</v>
       </c>
-      <c r="D7" s="33" t="str">
+      <c r="D7" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!D7</f>
         <v>3-sigma initial satellite velocity uncertainty</v>
       </c>
-      <c r="E7" s="78" t="n">
+      <c r="E7" s="55" t="n">
         <f aca="false">B7/3</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="68" t="str">
+      <c r="A8" s="11" t="str">
         <f aca="false">truthStateInitialUncertainty!A8</f>
         <v>sig_ax</v>
       </c>
-      <c r="B8" s="33" t="n">
+      <c r="B8" s="13" t="n">
         <f aca="false">truthStateInitialUncertainty!B8</f>
         <v>0.0005</v>
       </c>
-      <c r="C8" s="33" t="str">
+      <c r="C8" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!C8</f>
         <v>rad</v>
       </c>
-      <c r="D8" s="33" t="str">
+      <c r="D8" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!D8</f>
         <v>3-sigma initial satellite orientation uncertainty</v>
       </c>
-      <c r="E8" s="78" t="n">
+      <c r="E8" s="55" t="n">
         <f aca="false">B8/3</f>
         <v>0.000166666666666667</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="68" t="str">
+      <c r="A9" s="11" t="str">
         <f aca="false">truthStateInitialUncertainty!A9</f>
         <v>sig_ay</v>
       </c>
-      <c r="B9" s="33" t="n">
+      <c r="B9" s="13" t="n">
         <f aca="false">truthStateInitialUncertainty!B9</f>
         <v>0.0005</v>
       </c>
-      <c r="C9" s="33" t="str">
+      <c r="C9" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!C9</f>
         <v>rad</v>
       </c>
-      <c r="D9" s="33" t="str">
+      <c r="D9" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!D9</f>
         <v>3-sigma initial satellite orientation uncertainty</v>
       </c>
-      <c r="E9" s="78" t="n">
+      <c r="E9" s="55" t="n">
         <f aca="false">B9/3</f>
         <v>0.000166666666666667</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="68" t="str">
+      <c r="A10" s="11" t="str">
         <f aca="false">truthStateInitialUncertainty!A10</f>
         <v>sig_az</v>
       </c>
-      <c r="B10" s="33" t="n">
+      <c r="B10" s="13" t="n">
         <f aca="false">truthStateInitialUncertainty!B10</f>
         <v>0.0005</v>
       </c>
-      <c r="C10" s="33" t="str">
+      <c r="C10" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!C10</f>
         <v>rad</v>
       </c>
-      <c r="D10" s="33" t="str">
+      <c r="D10" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!D10</f>
         <v>3-sigma initial satellite orientation uncertainty</v>
       </c>
-      <c r="E10" s="78" t="n">
+      <c r="E10" s="55" t="n">
         <f aca="false">B10/3</f>
         <v>0.000166666666666667</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="68" t="str">
+      <c r="A11" s="11" t="str">
         <f aca="false">truthStateInitialUncertainty!A11</f>
         <v>sig_thstx</v>
       </c>
-      <c r="B11" s="33" t="n">
+      <c r="B11" s="13" t="n">
         <f aca="false">truthStateInitialUncertainty!B11</f>
         <v>20</v>
       </c>
-      <c r="C11" s="33" t="str">
+      <c r="C11" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!C11</f>
         <v>arcsec</v>
       </c>
-      <c r="D11" s="33" t="str">
+      <c r="D11" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!D11</f>
         <v>3-sigma initial star camera misalignment uncertainty</v>
       </c>
-      <c r="E11" s="78" t="n">
+      <c r="E11" s="55" t="n">
         <f aca="false">RADIANS(B11)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="68" t="str">
+      <c r="A12" s="11" t="str">
         <f aca="false">truthStateInitialUncertainty!A12</f>
         <v>sig_thsty</v>
       </c>
-      <c r="B12" s="33" t="n">
+      <c r="B12" s="13" t="n">
         <f aca="false">truthStateInitialUncertainty!B12</f>
         <v>20</v>
       </c>
-      <c r="C12" s="33" t="str">
+      <c r="C12" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!C12</f>
         <v>arcsec</v>
       </c>
-      <c r="D12" s="33" t="str">
+      <c r="D12" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!D12</f>
         <v>3-sigma initial star camera misalignment uncertainty</v>
       </c>
-      <c r="E12" s="78" t="n">
+      <c r="E12" s="55" t="n">
         <f aca="false">RADIANS(B12)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="68" t="str">
+      <c r="A13" s="11" t="str">
         <f aca="false">truthStateInitialUncertainty!A13</f>
         <v>sig_thstz</v>
       </c>
-      <c r="B13" s="33" t="n">
+      <c r="B13" s="13" t="n">
         <f aca="false">truthStateInitialUncertainty!B13</f>
         <v>20</v>
       </c>
-      <c r="C13" s="33" t="str">
+      <c r="C13" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!C13</f>
         <v>arcsec</v>
       </c>
-      <c r="D13" s="33" t="str">
+      <c r="D13" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!D13</f>
         <v>3-sigma initial star camera misalignment uncertainty</v>
       </c>
-      <c r="E13" s="78" t="n">
+      <c r="E13" s="55" t="n">
         <f aca="false">RADIANS(B13)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="68" t="str">
+      <c r="A14" s="11" t="str">
         <f aca="false">truthStateInitialUncertainty!A14</f>
         <v>sig_thcx</v>
       </c>
-      <c r="B14" s="33" t="n">
+      <c r="B14" s="13" t="n">
         <f aca="false">truthStateInitialUncertainty!B14</f>
         <v>20</v>
       </c>
-      <c r="C14" s="33" t="str">
+      <c r="C14" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!C14</f>
         <v>arcsec</v>
       </c>
-      <c r="D14" s="33" t="str">
+      <c r="D14" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!D14</f>
         <v>3-sigma initial terrain camera misalignment uncertainty</v>
       </c>
-      <c r="E14" s="78" t="n">
+      <c r="E14" s="55" t="n">
         <f aca="false">RADIANS(B14)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="68" t="str">
+      <c r="A15" s="11" t="str">
         <f aca="false">truthStateInitialUncertainty!A15</f>
         <v>sig_thcy</v>
       </c>
-      <c r="B15" s="33" t="n">
+      <c r="B15" s="13" t="n">
         <f aca="false">truthStateInitialUncertainty!B15</f>
         <v>20</v>
       </c>
-      <c r="C15" s="33" t="str">
+      <c r="C15" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!C15</f>
         <v>arcsec</v>
       </c>
-      <c r="D15" s="33" t="str">
+      <c r="D15" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!D15</f>
         <v>3-sigma initial terrain camera misalignment uncertainty</v>
       </c>
-      <c r="E15" s="78" t="n">
+      <c r="E15" s="55" t="n">
         <f aca="false">RADIANS(B15)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="68" t="str">
+      <c r="A16" s="11" t="str">
         <f aca="false">truthStateInitialUncertainty!A16</f>
         <v>sig_thcz</v>
       </c>
-      <c r="B16" s="33" t="n">
+      <c r="B16" s="13" t="n">
         <f aca="false">truthStateInitialUncertainty!B16</f>
         <v>20</v>
       </c>
-      <c r="C16" s="33" t="str">
+      <c r="C16" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!C16</f>
         <v>arcsec</v>
       </c>
-      <c r="D16" s="33" t="str">
+      <c r="D16" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!D16</f>
         <v>3-sigma initial terrain camera misalignment uncertainty</v>
       </c>
-      <c r="E16" s="78" t="n">
+      <c r="E16" s="55" t="n">
         <f aca="false">RADIANS(B16)/3600/3</f>
         <v>3.23209120739691E-005</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="68" t="str">
+      <c r="A17" s="11" t="str">
         <f aca="false">truthStateInitialUncertainty!A17</f>
         <v>sig_gyrox</v>
       </c>
-      <c r="B17" s="33" t="n">
+      <c r="B17" s="13" t="n">
         <f aca="false">truthStateInitialUncertainty!B17</f>
         <v>5</v>
       </c>
-      <c r="C17" s="33" t="str">
+      <c r="C17" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!C17</f>
         <v>deg/hr</v>
       </c>
-      <c r="D17" s="33" t="str">
+      <c r="D17" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!D17</f>
         <v>3-sigma initial gyro bias uncertainty</v>
       </c>
-      <c r="E17" s="78" t="n">
+      <c r="E17" s="55" t="n">
         <f aca="false">RADIANS(B17)/hr2sec/3</f>
         <v>8.08022801849227E-006</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="68" t="str">
+      <c r="A18" s="11" t="str">
         <f aca="false">truthStateInitialUncertainty!A18</f>
         <v>sig_gyroy</v>
       </c>
-      <c r="B18" s="33" t="n">
+      <c r="B18" s="13" t="n">
         <f aca="false">truthStateInitialUncertainty!B18</f>
         <v>5</v>
       </c>
-      <c r="C18" s="33" t="str">
+      <c r="C18" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!C18</f>
         <v>deg/hr</v>
       </c>
-      <c r="D18" s="33" t="str">
+      <c r="D18" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!D18</f>
         <v>3-sigma initial gyro bias uncertainty</v>
       </c>
-      <c r="E18" s="78" t="n">
+      <c r="E18" s="55" t="n">
         <f aca="false">RADIANS(B18)/hr2sec/3</f>
         <v>8.08022801849227E-006</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="35" t="str">
+      <c r="A19" s="28" t="str">
         <f aca="false">truthStateInitialUncertainty!A19</f>
         <v>sig_gyroz</v>
       </c>
-      <c r="B19" s="37" t="n">
+      <c r="B19" s="30" t="n">
         <f aca="false">truthStateInitialUncertainty!B19</f>
         <v>5</v>
       </c>
-      <c r="C19" s="37" t="str">
+      <c r="C19" s="30" t="str">
         <f aca="false">truthStateInitialUncertainty!C19</f>
         <v>deg/hr</v>
       </c>
-      <c r="D19" s="37" t="str">
+      <c r="D19" s="30" t="str">
         <f aca="false">truthStateInitialUncertainty!D19</f>
         <v>3-sigma initial gyro bias uncertainty</v>
       </c>
-      <c r="E19" s="79" t="n">
+      <c r="E19" s="56" t="n">
         <f aca="false">RADIANS(B19)/hr2sec/3</f>
         <v>8.08022801849227E-006</v>
       </c>
@@ -3854,8 +3824,8 @@
   </sheetPr>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3868,311 +3838,347 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="64" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="77" t="s">
+      <c r="A1" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="67" t="s">
+      <c r="E1" s="48" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="68" t="s">
-        <v>153</v>
-      </c>
-      <c r="B2" s="33" t="n">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="B2" s="57" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="57" t="s">
+        <v>160</v>
+      </c>
+      <c r="E2" s="55" t="n">
+        <f aca="false">B2</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3" s="58" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="58" t="s">
+        <v>160</v>
+      </c>
+      <c r="E3" s="55" t="n">
+        <f aca="false">B3</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B4" s="58" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="58" t="s">
+        <v>160</v>
+      </c>
+      <c r="E4" s="55" t="n">
+        <f aca="false">B4</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="B5" s="58" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="33"/>
-      <c r="E2" s="78" t="n">
-        <f aca="false">B2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="68" t="s">
-        <v>154</v>
-      </c>
-      <c r="B3" s="33" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="33"/>
-      <c r="E3" s="78" t="n">
-        <f aca="false">B3</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="68" t="s">
-        <v>155</v>
-      </c>
-      <c r="B4" s="33" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="33"/>
-      <c r="E4" s="78" t="n">
-        <f aca="false">B4</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="68" t="s">
-        <v>156</v>
-      </c>
-      <c r="B5" s="33" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="C5" s="33" t="str">
+      <c r="C5" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!C5</f>
         <v>m/sec</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="78" t="n">
+      <c r="D5" s="58" t="s">
+        <v>164</v>
+      </c>
+      <c r="E5" s="55" t="n">
         <f aca="false">B5</f>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="68" t="s">
-        <v>157</v>
-      </c>
-      <c r="B6" s="33" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="C6" s="33" t="str">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="B6" s="58" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!C6</f>
         <v>m/sec</v>
       </c>
-      <c r="D6" s="33"/>
-      <c r="E6" s="78" t="n">
+      <c r="D6" s="58" t="s">
+        <v>164</v>
+      </c>
+      <c r="E6" s="55" t="n">
         <f aca="false">B6</f>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="68" t="s">
-        <v>158</v>
-      </c>
-      <c r="B7" s="33" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="C7" s="33" t="str">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B7" s="58" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" s="13" t="str">
         <f aca="false">truthStateInitialUncertainty!C7</f>
         <v>m/sec</v>
       </c>
-      <c r="D7" s="33"/>
-      <c r="E7" s="78" t="n">
+      <c r="D7" s="58" t="s">
+        <v>164</v>
+      </c>
+      <c r="E7" s="55" t="n">
         <f aca="false">B7</f>
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="68" t="s">
-        <v>159</v>
-      </c>
-      <c r="B8" s="33" t="n">
-        <v>0.11</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>160</v>
-      </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="78" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="B8" s="58" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="D8" s="58" t="s">
+        <v>169</v>
+      </c>
+      <c r="E8" s="55" t="n">
         <f aca="false">RADIANS(B8)</f>
-        <v>0.00191986217719376</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="68" t="s">
-        <v>161</v>
-      </c>
-      <c r="B9" s="33" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="C9" s="33" t="s">
-        <v>62</v>
-      </c>
-      <c r="D9" s="33"/>
-      <c r="E9" s="78" t="n">
+        <v>0.000174532925199433</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B9" s="58" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="58" t="s">
+        <v>169</v>
+      </c>
+      <c r="E9" s="55" t="n">
         <f aca="false">RADIANS(B9)</f>
-        <v>0.00383972435438752</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="68" t="s">
-        <v>162</v>
-      </c>
-      <c r="B10" s="33" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="C10" s="33" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" s="33"/>
-      <c r="E10" s="78" t="n">
+        <v>0.000349065850398866</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="B10" s="58" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="58" t="s">
+        <v>169</v>
+      </c>
+      <c r="E10" s="55" t="n">
         <f aca="false">RADIANS(B10)</f>
-        <v>0.00575958653158129</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="68" t="s">
-        <v>163</v>
-      </c>
-      <c r="B11" s="33" t="n">
+        <v>0.000523598775598299</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B11" s="59" t="n">
         <v>0.001</v>
       </c>
-      <c r="C11" s="33" t="s">
+      <c r="C11" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="33"/>
-      <c r="E11" s="78" t="n">
+      <c r="D11" s="59" t="s">
+        <v>173</v>
+      </c>
+      <c r="E11" s="55" t="n">
         <f aca="false">g2mps2*B11</f>
         <v>0.00981</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="68" t="s">
-        <v>164</v>
-      </c>
-      <c r="B12" s="33" t="n">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="B12" s="59" t="n">
         <v>0.002</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="33"/>
-      <c r="E12" s="78" t="n">
+      <c r="D12" s="59" t="s">
+        <v>173</v>
+      </c>
+      <c r="E12" s="55" t="n">
         <f aca="false">g2mps2*B12</f>
         <v>0.01962</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="68" t="s">
-        <v>165</v>
-      </c>
-      <c r="B13" s="33" t="n">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="B13" s="59" t="n">
         <v>0.003</v>
       </c>
-      <c r="C13" s="33" t="s">
+      <c r="C13" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="33"/>
-      <c r="E13" s="78" t="n">
+      <c r="D13" s="59" t="s">
+        <v>173</v>
+      </c>
+      <c r="E13" s="55" t="n">
         <f aca="false">g2mps2*B13</f>
         <v>0.02943</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="68" t="s">
-        <v>166</v>
-      </c>
-      <c r="B14" s="33" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="C14" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="D14" s="33"/>
-      <c r="E14" s="78" t="n">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="B14" s="58" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="58" t="s">
+        <v>177</v>
+      </c>
+      <c r="E14" s="55" t="n">
         <f aca="false">RADIANS(B14)/hr2sec</f>
-        <v>5.3329504922049E-006</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="68" t="s">
-        <v>167</v>
-      </c>
-      <c r="B15" s="33" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="C15" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="D15" s="33"/>
-      <c r="E15" s="78" t="n">
+        <v>4.84813681109536E-006</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="B15" s="58" t="n">
+        <v>2</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="58" t="s">
+        <v>177</v>
+      </c>
+      <c r="E15" s="55" t="n">
         <f aca="false">RADIANS(B15)/hr2sec</f>
-        <v>5.81776417331443E-006</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="68" t="s">
-        <v>168</v>
-      </c>
-      <c r="B16" s="33" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="C16" s="33" t="s">
-        <v>73</v>
-      </c>
-      <c r="D16" s="33"/>
-      <c r="E16" s="78" t="n">
+        <v>9.69627362219072E-006</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="B16" s="58" t="n">
+        <v>3</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="58" t="s">
+        <v>177</v>
+      </c>
+      <c r="E16" s="55" t="n">
         <f aca="false">RADIANS(B16)/hr2sec</f>
-        <v>6.30257785442397E-006</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="68" t="s">
-        <v>169</v>
-      </c>
-      <c r="B17" s="33" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="C17" s="33" t="s">
+        <v>1.45444104332861E-005</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="B17" s="58" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="C17" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="33"/>
-      <c r="E17" s="78" t="n">
+      <c r="D17" s="58" t="s">
+        <v>181</v>
+      </c>
+      <c r="E17" s="55" t="n">
         <f aca="false">B17</f>
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="68" t="s">
-        <v>170</v>
-      </c>
-      <c r="B18" s="33" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="C18" s="33" t="s">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="B18" s="58" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="C18" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="33"/>
-      <c r="E18" s="78" t="n">
+      <c r="D18" s="58" t="s">
+        <v>181</v>
+      </c>
+      <c r="E18" s="55" t="n">
         <f aca="false">B18</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="B19" s="37" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="C19" s="37" t="s">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="28" t="s">
+        <v>183</v>
+      </c>
+      <c r="B19" s="60" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="C19" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="37"/>
-      <c r="E19" s="79" t="n">
+      <c r="D19" s="60" t="s">
+        <v>181</v>
+      </c>
+      <c r="E19" s="56" t="n">
         <f aca="false">B19</f>
-        <v>0.03</v>
+        <v>0.33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
code working, the estimated state diverges. the true state looks good
</commit_message>
<xml_diff>
--- a/config_randy.xlsx
+++ b/config_randy.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -775,7 +775,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="60">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1005,10 +1005,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1099,7 +1095,7 @@
   </sheetPr>
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -1136,7 +1132,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="8" t="n">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>6</v>
@@ -1146,7 +1142,7 @@
       </c>
       <c r="E2" s="10" t="n">
         <f aca="false">B2</f>
-        <v>0.01</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1281,7 +1277,7 @@
         <v>23</v>
       </c>
       <c r="B10" s="15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>13</v>
@@ -1291,7 +1287,7 @@
       </c>
       <c r="E10" s="14" t="n">
         <f aca="false">B10</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1299,7 +1295,7 @@
         <v>25</v>
       </c>
       <c r="B11" s="15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>13</v>
@@ -1309,7 +1305,7 @@
       </c>
       <c r="E11" s="14" t="n">
         <f aca="false">B11</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1676,8 +1672,8 @@
   </sheetPr>
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1784,7 +1780,7 @@
         <v>70</v>
       </c>
       <c r="B6" s="33" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C6" s="34" t="s">
         <v>68</v>
@@ -1794,7 +1790,7 @@
       </c>
       <c r="E6" s="35" t="n">
         <f aca="false">RADIANS(B6)</f>
-        <v>0.0872664625997165</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3824,7 +3820,7 @@
   </sheetPr>
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
@@ -4023,13 +4019,13 @@
       <c r="A11" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="B11" s="59" t="n">
+      <c r="B11" s="58" t="n">
         <v>0.001</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="59" t="s">
+      <c r="D11" s="58" t="s">
         <v>173</v>
       </c>
       <c r="E11" s="55" t="n">
@@ -4041,13 +4037,13 @@
       <c r="A12" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="B12" s="59" t="n">
+      <c r="B12" s="58" t="n">
         <v>0.002</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="59" t="s">
+      <c r="D12" s="58" t="s">
         <v>173</v>
       </c>
       <c r="E12" s="55" t="n">
@@ -4059,13 +4055,13 @@
       <c r="A13" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="B13" s="59" t="n">
+      <c r="B13" s="58" t="n">
         <v>0.003</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="59" t="s">
+      <c r="D13" s="58" t="s">
         <v>173</v>
       </c>
       <c r="E13" s="55" t="n">
@@ -4167,13 +4163,13 @@
       <c r="A19" s="28" t="s">
         <v>183</v>
       </c>
-      <c r="B19" s="60" t="n">
+      <c r="B19" s="59" t="n">
         <v>0.33</v>
       </c>
       <c r="C19" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="60" t="s">
+      <c r="D19" s="59" t="s">
         <v>181</v>
       </c>
       <c r="E19" s="56" t="n">

</xml_diff>